<commit_message>
Working on Jorge comments
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{524200B2-28BA-B543-8538-4DD47AB1ED5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3318835-D22A-A94C-BED0-F95B52692C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="31240" windowHeight="28040" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="142">
   <si>
     <t>Commenter</t>
   </si>
@@ -729,6 +729,21 @@
       </rPr>
       <t xml:space="preserve"> is to produce energy, but this is not the case for a material. Moreover, there are very clear examples of this. For instance, the exergy of aluminum is very high (it reacts strongly with the environment) compared to gold. This might suggest that aluminum production processes are more efficient than those of gold, which does not necessarily hold true. Therefore, I think it is important to retain mass-based values alongside exergy so as not to lose this perspective.</t>
     </r>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>Added EROI to the sentence in question.</t>
+  </si>
+  <si>
+    <t>Delete the phrase "and in response to the above reasons,"</t>
+  </si>
+  <si>
+    <t>No changes. Jorge is talking about the exergy of the material output from a process. We are speaking about the efficiency of that process to upgrade the exergy of the material being processed.</t>
+  </si>
+  <si>
+    <t>Added a limitations section to the Discussion. We can include additional limitations as we see fit.</t>
   </si>
 </sst>
 </file>
@@ -819,7 +834,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -844,6 +859,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -858,7 +879,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -878,9 +899,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -888,9 +906,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -901,9 +916,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -952,6 +964,25 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1570,19 +1601,22 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="22" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.1640625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="61.1640625" style="30" customWidth="1"/>
+    <col min="6" max="6" width="48.33203125" style="3" customWidth="1"/>
     <col min="8" max="8" width="66.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="31"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1594,10 +1628,10 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="23" t="s">
+      <c r="E1" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
@@ -1611,7 +1645,7 @@
       </c>
     </row>
     <row r="2" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B2" s="1"/>
@@ -1619,20 +1653,20 @@
       <c r="D2" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="24" t="s">
+      <c r="E2" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1"/>
+      <c r="F2" s="4"/>
       <c r="G2" s="1"/>
       <c r="H2" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="I2" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A3" s="18" t="s">
+      <c r="A3" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1"/>
@@ -1640,20 +1674,20 @@
       <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="24" t="s">
+      <c r="E3" s="21" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1"/>
+      <c r="F3" s="4"/>
       <c r="G3" s="1"/>
       <c r="H3" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="I3" s="2" t="s">
+      <c r="I3" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="18" t="s">
+      <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B4" s="1"/>
@@ -1661,20 +1695,20 @@
       <c r="D4" s="1">
         <v>48</v>
       </c>
-      <c r="E4" s="24" t="s">
+      <c r="E4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="1"/>
+      <c r="F4" s="4"/>
       <c r="G4" s="1"/>
       <c r="H4" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="2" t="s">
+      <c r="I4" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="18" t="s">
+      <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="1"/>
@@ -1682,18 +1716,18 @@
       <c r="D5" s="1">
         <v>74</v>
       </c>
-      <c r="E5" s="24" t="s">
+      <c r="E5" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="1"/>
+      <c r="F5" s="4"/>
       <c r="G5" s="1"/>
       <c r="H5" s="4"/>
-      <c r="I5" s="2" t="s">
+      <c r="I5" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="18" t="s">
+      <c r="A6" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="1"/>
@@ -1701,18 +1735,18 @@
       <c r="D6" s="1">
         <v>151</v>
       </c>
-      <c r="E6" s="24" t="s">
+      <c r="E6" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="1"/>
+      <c r="F6" s="4"/>
       <c r="G6" s="1"/>
       <c r="H6" s="4"/>
-      <c r="I6" s="2" t="s">
+      <c r="I6" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="18" t="s">
+      <c r="A7" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="1"/>
@@ -1720,18 +1754,18 @@
       <c r="D7" s="1">
         <v>159</v>
       </c>
-      <c r="E7" s="24" t="s">
+      <c r="E7" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="4"/>
       <c r="G7" s="1"/>
       <c r="H7" s="4"/>
-      <c r="I7" s="2" t="s">
+      <c r="I7" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="18" t="s">
+      <c r="A8" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="1"/>
@@ -1739,18 +1773,18 @@
       <c r="D8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="E8" s="21" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="1"/>
+      <c r="F8" s="4"/>
       <c r="G8" s="1"/>
       <c r="H8" s="4"/>
-      <c r="I8" s="2" t="s">
+      <c r="I8" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="18" t="s">
+      <c r="A9" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1"/>
@@ -1758,18 +1792,18 @@
       <c r="D9" s="1">
         <v>218</v>
       </c>
-      <c r="E9" s="24" t="s">
+      <c r="E9" s="21" t="s">
         <v>131</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="4"/>
       <c r="G9" s="1"/>
       <c r="H9" s="4"/>
-      <c r="I9" s="2" t="s">
+      <c r="I9" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="18" t="s">
+      <c r="A10" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B10" s="1"/>
@@ -1777,18 +1811,18 @@
       <c r="D10" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="24" t="s">
+      <c r="E10" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="4"/>
       <c r="G10" s="1"/>
       <c r="H10" s="4"/>
-      <c r="I10" s="2" t="s">
+      <c r="I10" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="18" t="s">
+      <c r="A11" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="1"/>
@@ -1796,20 +1830,20 @@
       <c r="D11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="24" t="s">
+      <c r="E11" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="1"/>
+      <c r="F11" s="4"/>
       <c r="G11" s="1"/>
       <c r="H11" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="2" t="s">
+      <c r="I11" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="18" t="s">
+      <c r="A12" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1"/>
@@ -1817,18 +1851,18 @@
       <c r="D12" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="E12" s="21" t="s">
         <v>132</v>
       </c>
-      <c r="F12" s="1"/>
+      <c r="F12" s="4"/>
       <c r="G12" s="1"/>
       <c r="H12" s="4"/>
-      <c r="I12" s="2" t="s">
+      <c r="I12" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="18" t="s">
+      <c r="A13" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B13" s="1"/>
@@ -1836,20 +1870,20 @@
       <c r="D13" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="1"/>
+      <c r="F13" s="4"/>
       <c r="G13" s="1"/>
       <c r="H13" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I13" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="18" t="s">
+      <c r="A14" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B14" s="1"/>
@@ -1857,18 +1891,18 @@
       <c r="D14" s="1">
         <v>438</v>
       </c>
-      <c r="E14" s="24" t="s">
+      <c r="E14" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="4"/>
       <c r="G14" s="1"/>
       <c r="H14" s="4"/>
-      <c r="I14" s="2" t="s">
+      <c r="I14" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A15" s="18" t="s">
+      <c r="A15" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="1"/>
@@ -1876,18 +1910,18 @@
       <c r="D15" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="1"/>
+      <c r="F15" s="4"/>
       <c r="G15" s="1"/>
       <c r="H15" s="4"/>
-      <c r="I15" s="2" t="s">
+      <c r="I15" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="18" t="s">
+      <c r="A16" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B16" s="1"/>
@@ -1895,20 +1929,20 @@
       <c r="D16" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="E16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="1"/>
+      <c r="F16" s="4"/>
       <c r="G16" s="1"/>
       <c r="H16" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="I16" s="2" t="s">
+      <c r="I16" s="1" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="18" t="s">
+      <c r="A17" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B17" s="1"/>
@@ -1916,18 +1950,18 @@
       <c r="D17" s="1">
         <v>487</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="E17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="1"/>
+      <c r="F17" s="4"/>
       <c r="G17" s="1"/>
       <c r="H17" s="4"/>
-      <c r="I17" s="2" t="s">
+      <c r="I17" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="18" t="s">
+      <c r="A18" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="1"/>
@@ -1935,18 +1969,18 @@
       <c r="D18" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="24" t="s">
+      <c r="E18" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="1"/>
+      <c r="F18" s="4"/>
       <c r="G18" s="1"/>
       <c r="H18" s="4"/>
-      <c r="I18" s="2" t="s">
+      <c r="I18" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" s="18" t="s">
+      <c r="A19" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B19" s="1"/>
@@ -1954,20 +1988,20 @@
       <c r="D19" s="1">
         <v>526</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="E19" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="4"/>
       <c r="G19" s="1"/>
       <c r="H19" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I19" s="2" t="s">
+      <c r="I19" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="18" t="s">
+      <c r="A20" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B20" s="1"/>
@@ -1975,18 +2009,18 @@
       <c r="D20" s="1">
         <v>527</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="E20" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="1"/>
+      <c r="F20" s="4"/>
       <c r="G20" s="1"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="2" t="s">
+      <c r="I20" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="18" t="s">
+      <c r="A21" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B21" s="1"/>
@@ -1994,18 +2028,18 @@
       <c r="D21" s="1">
         <v>533</v>
       </c>
-      <c r="E21" s="24" t="s">
+      <c r="E21" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="1"/>
+      <c r="F21" s="4"/>
       <c r="G21" s="1"/>
       <c r="H21" s="4"/>
-      <c r="I21" s="2" t="s">
+      <c r="I21" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="53" x14ac:dyDescent="0.2">
-      <c r="A22" s="18" t="s">
+      <c r="A22" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="1"/>
@@ -2013,18 +2047,18 @@
       <c r="D22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="24" t="s">
+      <c r="E22" s="21" t="s">
         <v>133</v>
       </c>
-      <c r="F22" s="1"/>
+      <c r="F22" s="4"/>
       <c r="G22" s="1"/>
       <c r="H22" s="4"/>
-      <c r="I22" s="2" t="s">
+      <c r="I22" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="119" x14ac:dyDescent="0.2">
-      <c r="A23" s="18" t="s">
+      <c r="A23" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="1"/>
@@ -2032,18 +2066,18 @@
       <c r="D23" s="1">
         <v>543</v>
       </c>
-      <c r="E23" s="24" t="s">
+      <c r="E23" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="1"/>
+      <c r="F23" s="4"/>
       <c r="G23" s="1"/>
       <c r="H23" s="4"/>
-      <c r="I23" s="2" t="s">
+      <c r="I23" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="18" t="s">
+      <c r="A24" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B24" s="1"/>
@@ -2051,20 +2085,20 @@
       <c r="D24" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="24" t="s">
+      <c r="E24" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="1"/>
+      <c r="F24" s="4"/>
       <c r="G24" s="1"/>
       <c r="H24" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="I24" s="2" t="s">
+      <c r="I24" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="1"/>
@@ -2072,18 +2106,18 @@
       <c r="D25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="21" t="s">
         <v>134</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="4"/>
       <c r="G25" s="1"/>
       <c r="H25" s="4"/>
-      <c r="I25" s="2" t="s">
+      <c r="I25" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="18" t="s">
+      <c r="A26" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B26" s="1"/>
@@ -2091,18 +2125,18 @@
       <c r="D26" s="1">
         <v>697</v>
       </c>
-      <c r="E26" s="24" t="s">
+      <c r="E26" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="4"/>
       <c r="G26" s="1"/>
       <c r="H26" s="4"/>
-      <c r="I26" s="2" t="s">
+      <c r="I26" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="18" t="s">
+      <c r="A27" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B27" s="1"/>
@@ -2110,18 +2144,18 @@
       <c r="D27" s="1">
         <v>718</v>
       </c>
-      <c r="E27" s="24" t="s">
+      <c r="E27" s="21" t="s">
         <v>135</v>
       </c>
-      <c r="F27" s="1"/>
+      <c r="F27" s="4"/>
       <c r="G27" s="1"/>
       <c r="H27" s="4"/>
-      <c r="I27" s="2" t="s">
+      <c r="I27" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="18" t="s">
+      <c r="A28" s="15" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="1"/>
@@ -2129,138 +2163,150 @@
       <c r="D28" s="1">
         <v>739</v>
       </c>
-      <c r="E28" s="24" t="s">
+      <c r="E28" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="1"/>
+      <c r="F28" s="4"/>
       <c r="G28" s="1"/>
       <c r="H28" s="4"/>
-      <c r="I28" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" s="8" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" s="19" t="s">
+      <c r="I28" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="36" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="5"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="5">
+      <c r="B29" s="33"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33">
         <v>18</v>
       </c>
-      <c r="E29" s="25" t="s">
+      <c r="E29" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="6" t="s">
+      <c r="F29" s="35" t="s">
+        <v>138</v>
+      </c>
+      <c r="G29" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="H29" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="I29" s="7" t="s">
+      <c r="I29" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A30" s="20" t="s">
+    <row r="30" spans="1:9" s="36" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A30" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="9">
+      <c r="B30" s="33"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33">
         <v>51</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="9"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="10"/>
-      <c r="I30" s="11" t="s">
+      <c r="F30" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="G30" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="H30" s="35"/>
+      <c r="I30" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="12" customFormat="1" ht="144" x14ac:dyDescent="0.2">
-      <c r="A31" s="20" t="s">
+    <row r="31" spans="1:9" s="36" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+      <c r="A31" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="9" t="s">
+      <c r="B31" s="33"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="26" t="s">
+      <c r="E31" s="37" t="s">
         <v>136</v>
       </c>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10" t="s">
+      <c r="F31" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="G31" s="33"/>
+      <c r="H31" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="11" t="s">
+      <c r="I31" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="12" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="20" t="s">
+    <row r="32" spans="1:9" s="10" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="9">
+      <c r="B32" s="8"/>
+      <c r="C32" s="8"/>
+      <c r="D32" s="8">
         <v>74</v>
       </c>
-      <c r="E32" s="27" t="s">
+      <c r="E32" s="24" t="s">
         <v>52</v>
       </c>
       <c r="F32" s="9"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="10"/>
-      <c r="I32" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:9" s="17" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="21" t="s">
+      <c r="G32" s="8"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="14"/>
-      <c r="C33" s="14"/>
-      <c r="D33" s="14" t="s">
+      <c r="B33" s="12"/>
+      <c r="C33" s="12"/>
+      <c r="D33" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="28" t="s">
+      <c r="E33" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="15" t="s">
+      <c r="F33" s="13"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="I33" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="34" spans="1:9" s="12" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A34" s="20" t="s">
+      <c r="I33" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" s="36" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A34" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9" t="s">
+      <c r="B34" s="33"/>
+      <c r="C34" s="33"/>
+      <c r="D34" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="26" t="s">
+      <c r="E34" s="37" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="10"/>
-      <c r="I34" s="11" t="s">
+      <c r="F34" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="G34" s="33"/>
+      <c r="H34" s="35"/>
+      <c r="I34" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="8" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A35" s="19" t="s">
+    <row r="35" spans="1:9" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A35" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B35" s="5"/>
@@ -2268,41 +2314,41 @@
       <c r="D35" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="29" t="s">
+      <c r="E35" s="26" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="5"/>
+      <c r="F35" s="6"/>
       <c r="G35" s="5"/>
       <c r="H35" s="6" t="s">
         <v>121</v>
       </c>
-      <c r="I35" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="12" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A36" s="20" t="s">
+      <c r="I35" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="10" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A36" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="9">
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8">
         <v>226</v>
       </c>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="24" t="s">
         <v>55</v>
       </c>
       <c r="F36" s="9"/>
-      <c r="G36" s="9"/>
-      <c r="H36" s="10" t="s">
+      <c r="G36" s="8"/>
+      <c r="H36" s="9" t="s">
         <v>122</v>
       </c>
-      <c r="I36" s="11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:9" s="8" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="19" t="s">
+      <c r="I36" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" s="7" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B37" s="5"/>
@@ -2310,81 +2356,85 @@
       <c r="D37" s="5">
         <v>254</v>
       </c>
-      <c r="E37" s="25" t="s">
+      <c r="E37" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="5"/>
+      <c r="F37" s="6"/>
       <c r="G37" s="5"/>
       <c r="H37" s="6"/>
-      <c r="I37" s="7" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:9" s="17" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A38" s="21" t="s">
+      <c r="I37" s="5" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" s="14" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A38" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="14"/>
-      <c r="C38" s="14"/>
-      <c r="D38" s="14" t="s">
+      <c r="B38" s="12"/>
+      <c r="C38" s="12"/>
+      <c r="D38" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="27" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="15" t="s">
+      <c r="F38" s="13"/>
+      <c r="G38" s="12"/>
+      <c r="H38" s="13" t="s">
         <v>123</v>
       </c>
-      <c r="I38" s="16" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="39" spans="1:9" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A39" s="20" t="s">
+      <c r="I38" s="12" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" s="36" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A39" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="9"/>
-      <c r="C39" s="9"/>
-      <c r="D39" s="9" t="s">
+      <c r="B39" s="33"/>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="26" t="s">
+      <c r="E39" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="F39" s="9"/>
-      <c r="G39" s="9"/>
-      <c r="H39" s="10" t="s">
+      <c r="F39" s="35" t="s">
+        <v>141</v>
+      </c>
+      <c r="G39" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="H39" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="I39" s="11" t="s">
+      <c r="I39" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="12" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A40" s="20" t="s">
+    <row r="40" spans="1:9" s="10" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A40" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="9" t="s">
+      <c r="B40" s="8"/>
+      <c r="C40" s="8"/>
+      <c r="D40" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="26" t="s">
+      <c r="E40" s="23" t="s">
         <v>61</v>
       </c>
       <c r="F40" s="9"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="10" t="s">
+      <c r="G40" s="8"/>
+      <c r="H40" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="I40" s="11" t="s">
+      <c r="I40" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="19" t="s">
+    <row r="41" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B41" s="5"/>
@@ -2392,20 +2442,20 @@
       <c r="D41" s="5">
         <v>425</v>
       </c>
-      <c r="E41" s="29" t="s">
+      <c r="E41" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="5"/>
+      <c r="F41" s="6"/>
       <c r="G41" s="5"/>
       <c r="H41" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="I41" s="7" t="s">
+      <c r="I41" s="5" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A42" s="18" t="s">
+      <c r="A42" s="15" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="1"/>
@@ -2413,39 +2463,39 @@
       <c r="D42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="31" t="s">
+      <c r="E42" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="F42" s="1"/>
+      <c r="F42" s="4"/>
       <c r="G42" s="1"/>
       <c r="H42" s="4"/>
-      <c r="I42" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="43" spans="1:9" s="12" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A43" s="20" t="s">
+      <c r="I42" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" s="10" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A43" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="9" t="s">
+      <c r="B43" s="8"/>
+      <c r="C43" s="8"/>
+      <c r="D43" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="26" t="s">
+      <c r="E43" s="23" t="s">
         <v>66</v>
       </c>
       <c r="F43" s="9"/>
-      <c r="G43" s="9"/>
-      <c r="H43" s="10" t="s">
+      <c r="G43" s="8"/>
+      <c r="H43" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="I43" s="11" t="s">
+      <c r="I43" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="8" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="19" t="s">
+    <row r="44" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="16" t="s">
         <v>42</v>
       </c>
       <c r="B44" s="5"/>
@@ -2453,62 +2503,62 @@
       <c r="D44" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="29" t="s">
+      <c r="E44" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="F44" s="5"/>
+      <c r="F44" s="6"/>
       <c r="G44" s="5"/>
       <c r="H44" s="6" t="s">
         <v>128</v>
       </c>
-      <c r="I44" s="7" t="s">
+      <c r="I44" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="12" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A45" s="20" t="s">
+    <row r="45" spans="1:9" s="10" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A45" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="9"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="9" t="s">
+      <c r="B45" s="8"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E45" s="26" t="s">
+      <c r="E45" s="23" t="s">
         <v>70</v>
       </c>
       <c r="F45" s="9"/>
-      <c r="G45" s="9"/>
-      <c r="H45" s="13" t="s">
+      <c r="G45" s="8"/>
+      <c r="H45" s="11" t="s">
         <v>71</v>
       </c>
-      <c r="I45" s="11" t="s">
+      <c r="I45" s="8" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="12" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A46" s="20" t="s">
+    <row r="46" spans="1:9" s="10" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A46" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9" t="s">
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="27" t="s">
+      <c r="E46" s="24" t="s">
         <v>73</v>
       </c>
       <c r="F46" s="9"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="10" t="s">
+      <c r="G46" s="8"/>
+      <c r="H46" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="I46" s="11" t="s">
+      <c r="I46" s="8" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="47" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B47" s="2" t="s">
@@ -2516,17 +2566,16 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="32" t="s">
+      <c r="E47" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="F47" s="2"/>
       <c r="G47" s="2"/>
-      <c r="I47" s="2" t="s">
+      <c r="I47" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="48" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A48" s="18" t="s">
+      <c r="A48" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B48" s="2">
@@ -2534,17 +2583,16 @@
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="32" t="s">
+      <c r="E48" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="F48" s="2"/>
       <c r="G48" s="2"/>
-      <c r="I48" s="2" t="s">
+      <c r="I48" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="49" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B49" s="2">
@@ -2552,17 +2600,16 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="32" t="s">
+      <c r="E49" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="F49" s="2"/>
       <c r="G49" s="2"/>
-      <c r="I49" s="2" t="s">
+      <c r="I49" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="18" t="s">
+      <c r="A50" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B50" s="2" t="s">
@@ -2570,17 +2617,16 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="32" t="s">
+      <c r="E50" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="F50" s="2"/>
       <c r="G50" s="2"/>
-      <c r="I50" s="2" t="s">
+      <c r="I50" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="51" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B51" s="2" t="s">
@@ -2588,17 +2634,16 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="32" t="s">
+      <c r="E51" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="F51" s="2"/>
       <c r="G51" s="2"/>
-      <c r="I51" s="2" t="s">
+      <c r="I51" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="18" t="s">
+      <c r="A52" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B52" s="2" t="s">
@@ -2608,17 +2653,16 @@
       <c r="D52" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E52" s="32" t="s">
+      <c r="E52" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="F52" s="2"/>
       <c r="G52" s="2"/>
-      <c r="I52" s="2" t="s">
+      <c r="I52" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="53" spans="1:9" ht="240" x14ac:dyDescent="0.2">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B53" s="2" t="s">
@@ -2628,17 +2672,16 @@
       <c r="D53" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E53" s="32" t="s">
+      <c r="E53" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="F53" s="2"/>
       <c r="G53" s="2"/>
-      <c r="I53" s="2" t="s">
+      <c r="I53" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="18" t="s">
+      <c r="A54" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B54" s="2" t="s">
@@ -2648,17 +2691,16 @@
       <c r="D54" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E54" s="32" t="s">
+      <c r="E54" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="F54" s="2"/>
       <c r="G54" s="2"/>
-      <c r="I54" s="2" t="s">
+      <c r="I54" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="18" t="s">
+      <c r="A55" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B55" s="2" t="s">
@@ -2666,17 +2708,16 @@
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="32" t="s">
+      <c r="E55" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="F55" s="2"/>
       <c r="G55" s="2"/>
-      <c r="I55" s="2" t="s">
+      <c r="I55" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="18" t="s">
+      <c r="A56" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B56" s="2" t="s">
@@ -2684,17 +2725,16 @@
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="32" t="s">
+      <c r="E56" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="F56" s="2"/>
       <c r="G56" s="2"/>
-      <c r="I56" s="2" t="s">
+      <c r="I56" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="57" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A57" s="18" t="s">
+      <c r="A57" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -2702,17 +2742,16 @@
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="32" t="s">
+      <c r="E57" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="F57" s="2"/>
       <c r="G57" s="2"/>
-      <c r="I57" s="2" t="s">
+      <c r="I57" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="18" t="s">
+      <c r="A58" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B58" s="2" t="s">
@@ -2722,19 +2761,19 @@
       <c r="D58" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E58" s="32" t="s">
+      <c r="E58" s="29" t="s">
         <v>96</v>
       </c>
-      <c r="F58" s="2" t="s">
+      <c r="F58" s="3" t="s">
         <v>88</v>
       </c>
       <c r="G58" s="2"/>
-      <c r="I58" s="2" t="s">
+      <c r="I58" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="18" t="s">
+      <c r="A59" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B59" s="2" t="s">
@@ -2744,17 +2783,16 @@
       <c r="D59" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E59" s="32" t="s">
+      <c r="E59" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="F59" s="2"/>
       <c r="G59" s="2"/>
-      <c r="I59" s="2" t="s">
+      <c r="I59" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B60" s="2" t="s">
@@ -2764,17 +2802,16 @@
       <c r="D60" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E60" s="32" t="s">
+      <c r="E60" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="F60" s="2"/>
       <c r="G60" s="2"/>
-      <c r="I60" s="2" t="s">
+      <c r="I60" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B61" s="2" t="s">
@@ -2784,17 +2821,16 @@
       <c r="D61" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E61" s="32" t="s">
+      <c r="E61" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="F61" s="2"/>
       <c r="G61" s="2"/>
-      <c r="I61" s="2" t="s">
+      <c r="I61" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="18" t="s">
+      <c r="A62" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B62" s="2">
@@ -2804,17 +2840,16 @@
       <c r="D62" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E62" s="32" t="s">
+      <c r="E62" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="F62" s="2"/>
       <c r="G62" s="2"/>
-      <c r="I62" s="2" t="s">
+      <c r="I62" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="18" t="s">
+      <c r="A63" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B63" s="2" t="s">
@@ -2824,17 +2859,16 @@
       <c r="D63" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E63" s="32" t="s">
+      <c r="E63" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="F63" s="2"/>
       <c r="G63" s="2"/>
-      <c r="I63" s="2" t="s">
+      <c r="I63" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="18" t="s">
+      <c r="A64" s="15" t="s">
         <v>74</v>
       </c>
       <c r="B64" s="2">
@@ -2844,12 +2878,11 @@
       <c r="D64" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E64" s="32" t="s">
+      <c r="E64" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="F64" s="2"/>
       <c r="G64" s="2"/>
-      <c r="I64" s="2" t="s">
+      <c r="I64" s="1" t="s">
         <v>78</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update by Jorge's comments.
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3318835-D22A-A94C-BED0-F95B52692C44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE5CBA7-EF52-1541-84CB-20EB2A0B3B51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="31240" windowHeight="28040" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
@@ -1602,7 +1602,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H40" sqref="H40"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added text about exergy costs.
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E4170D-8BDB-C740-BD3D-23A425DA9D16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B718719-ADD4-894A-820D-926C1E5C9F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="31240" windowHeight="28040" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="147">
   <si>
     <t>Commenter</t>
   </si>
@@ -750,6 +750,15 @@
   </si>
   <si>
     <t xml:space="preserve">Changed from "quality" to "usefulness". </t>
+  </si>
+  <si>
+    <t>Added a sentence to the caption.</t>
+  </si>
+  <si>
+    <t>Moved the cut line.</t>
+  </si>
+  <si>
+    <t>matrix equation --&gt; vector difference</t>
   </si>
 </sst>
 </file>
@@ -1610,8 +1619,8 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A11" sqref="A11:XFD11"/>
+      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1838,43 +1847,51 @@
         <v>78</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="15" t="s">
+    <row r="11" spans="1:9" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1" t="s">
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="21" t="s">
+      <c r="E11" s="38" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="4" t="s">
+      <c r="F11" s="35" t="s">
+        <v>144</v>
+      </c>
+      <c r="G11" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="H11" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="I11" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="15" t="s">
+    <row r="12" spans="1:9" s="36" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1" t="s">
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="21" t="s">
+      <c r="E12" s="38" t="s">
         <v>132</v>
       </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="1" t="s">
+      <c r="F12" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="G12" s="33" t="s">
+        <v>137</v>
+      </c>
+      <c r="H12" s="35"/>
+      <c r="I12" s="33" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1949,8 +1966,12 @@
       <c r="E16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="1"/>
+      <c r="F16" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>137</v>
+      </c>
       <c r="H16" s="4" t="s">
         <v>117</v>
       </c>

</xml_diff>

<commit_message>
Working on Jorge's comments about concentration exergy
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B718719-ADD4-894A-820D-926C1E5C9F6E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6EAF25-B742-D54B-ADB1-FC89240CF071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="31240" windowHeight="28040" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="36900" windowHeight="28040" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Review 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="148">
   <si>
     <t>Commenter</t>
   </si>
@@ -432,9 +432,6 @@
   </si>
   <si>
     <t>Double-check with comments from Tania</t>
-  </si>
-  <si>
-    <t>First step (ES): verify that we think our equations are correct. Second step: discuss with Jorge the reference state for concentration exergy. Thirdy step: get with Jorge to discuss if we think our equations are correct.</t>
   </si>
   <si>
     <t>Add a limitiations section(in discussion)  and discuss material infrastructure in that sections.</t>
@@ -759,6 +756,12 @@
   </si>
   <si>
     <t>matrix equation --&gt; vector difference</t>
+  </si>
+  <si>
+    <t>Added a paragraph in the dicussion about concentration exergy quantifying assembly processes in manufacturing.</t>
+  </si>
+  <si>
+    <t>First step (ES): verify that we think our equations are correct. Second step: discuss with Jorge the reference state for concentration exergy. Third step: get with Jorge to discuss if we think our equations are correct.</t>
   </si>
 </sst>
 </file>
@@ -894,7 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1001,6 +1004,21 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1619,8 +1637,8 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F17" sqref="F17"/>
+      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1629,6 +1647,7 @@
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61.1640625" style="30" customWidth="1"/>
     <col min="6" max="6" width="48.33203125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" style="39" customWidth="1"/>
     <col min="8" max="8" width="66.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="31"/>
   </cols>
@@ -1652,7 +1671,7 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="39" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -1675,10 +1694,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="G2" s="33" t="s">
-        <v>137</v>
+        <v>142</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="H2" s="35" t="s">
         <v>113</v>
@@ -1700,7 +1719,6 @@
         <v>12</v>
       </c>
       <c r="F3" s="4"/>
-      <c r="G3" s="1"/>
       <c r="H3" s="4" t="s">
         <v>114</v>
       </c>
@@ -1721,10 +1739,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="G4" s="33" t="s">
-        <v>137</v>
+        <v>142</v>
+      </c>
+      <c r="G4" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="H4" s="35" t="s">
         <v>113</v>
@@ -1746,7 +1764,6 @@
         <v>14</v>
       </c>
       <c r="F5" s="4"/>
-      <c r="G5" s="1"/>
       <c r="H5" s="4"/>
       <c r="I5" s="1" t="s">
         <v>78</v>
@@ -1765,7 +1782,6 @@
         <v>16</v>
       </c>
       <c r="F6" s="4"/>
-      <c r="G6" s="1"/>
       <c r="H6" s="4"/>
       <c r="I6" s="1" t="s">
         <v>78</v>
@@ -1781,10 +1797,9 @@
         <v>159</v>
       </c>
       <c r="E7" s="21" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F7" s="4"/>
-      <c r="G7" s="1"/>
       <c r="H7" s="4"/>
       <c r="I7" s="1" t="s">
         <v>78</v>
@@ -1803,7 +1818,6 @@
         <v>17</v>
       </c>
       <c r="F8" s="4"/>
-      <c r="G8" s="1"/>
       <c r="H8" s="4"/>
       <c r="I8" s="1" t="s">
         <v>78</v>
@@ -1819,10 +1833,9 @@
         <v>218</v>
       </c>
       <c r="E9" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F9" s="4"/>
-      <c r="G9" s="1"/>
       <c r="H9" s="4"/>
       <c r="I9" s="1" t="s">
         <v>78</v>
@@ -1841,7 +1854,6 @@
         <v>18</v>
       </c>
       <c r="F10" s="4"/>
-      <c r="G10" s="1"/>
       <c r="H10" s="4"/>
       <c r="I10" s="1" t="s">
         <v>78</v>
@@ -1860,10 +1872,10 @@
         <v>20</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="G11" s="33" t="s">
-        <v>137</v>
+        <v>143</v>
+      </c>
+      <c r="G11" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="H11" s="35" t="s">
         <v>115</v>
@@ -1882,13 +1894,13 @@
         <v>21</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>145</v>
-      </c>
-      <c r="G12" s="33" t="s">
-        <v>137</v>
+        <v>144</v>
+      </c>
+      <c r="G12" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="H12" s="35"/>
       <c r="I12" s="33" t="s">
@@ -1908,7 +1920,6 @@
         <v>23</v>
       </c>
       <c r="F13" s="4"/>
-      <c r="G13" s="1"/>
       <c r="H13" s="4" t="s">
         <v>116</v>
       </c>
@@ -1929,7 +1940,6 @@
         <v>24</v>
       </c>
       <c r="F14" s="4"/>
-      <c r="G14" s="1"/>
       <c r="H14" s="4"/>
       <c r="I14" s="1" t="s">
         <v>78</v>
@@ -1948,34 +1958,33 @@
         <v>25</v>
       </c>
       <c r="F15" s="4"/>
-      <c r="G15" s="1"/>
       <c r="H15" s="4"/>
       <c r="I15" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="15" t="s">
+    <row r="16" spans="1:9" s="36" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1" t="s">
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="21" t="s">
+      <c r="E16" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>146</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="H16" s="4" t="s">
+      <c r="F16" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="G16" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="H16" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="33" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1992,7 +2001,6 @@
         <v>29</v>
       </c>
       <c r="F17" s="4"/>
-      <c r="G17" s="1"/>
       <c r="H17" s="4"/>
       <c r="I17" s="1" t="s">
         <v>78</v>
@@ -2011,7 +2019,6 @@
         <v>31</v>
       </c>
       <c r="F18" s="4"/>
-      <c r="G18" s="1"/>
       <c r="H18" s="4"/>
       <c r="I18" s="1" t="s">
         <v>78</v>
@@ -2030,7 +2037,6 @@
         <v>32</v>
       </c>
       <c r="F19" s="4"/>
-      <c r="G19" s="1"/>
       <c r="H19" s="4" t="s">
         <v>118</v>
       </c>
@@ -2051,7 +2057,6 @@
         <v>33</v>
       </c>
       <c r="F20" s="4"/>
-      <c r="G20" s="1"/>
       <c r="H20" s="4"/>
       <c r="I20" s="1" t="s">
         <v>78</v>
@@ -2070,7 +2075,6 @@
         <v>34</v>
       </c>
       <c r="F21" s="4"/>
-      <c r="G21" s="1"/>
       <c r="H21" s="4"/>
       <c r="I21" s="1" t="s">
         <v>78</v>
@@ -2086,10 +2090,9 @@
         <v>35</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F22" s="4"/>
-      <c r="G22" s="1"/>
       <c r="H22" s="4"/>
       <c r="I22" s="1" t="s">
         <v>78</v>
@@ -2108,7 +2111,6 @@
         <v>38</v>
       </c>
       <c r="F23" s="4"/>
-      <c r="G23" s="1"/>
       <c r="H23" s="4"/>
       <c r="I23" s="1" t="s">
         <v>78</v>
@@ -2127,7 +2129,6 @@
         <v>39</v>
       </c>
       <c r="F24" s="4"/>
-      <c r="G24" s="1"/>
       <c r="H24" s="4" t="s">
         <v>118</v>
       </c>
@@ -2145,10 +2146,9 @@
         <v>37</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F25" s="4"/>
-      <c r="G25" s="1"/>
       <c r="H25" s="4"/>
       <c r="I25" s="1" t="s">
         <v>78</v>
@@ -2167,7 +2167,6 @@
         <v>40</v>
       </c>
       <c r="F26" s="4"/>
-      <c r="G26" s="1"/>
       <c r="H26" s="4"/>
       <c r="I26" s="1" t="s">
         <v>78</v>
@@ -2183,10 +2182,9 @@
         <v>718</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F27" s="4"/>
-      <c r="G27" s="1"/>
       <c r="H27" s="4"/>
       <c r="I27" s="1" t="s">
         <v>78</v>
@@ -2205,7 +2203,6 @@
         <v>41</v>
       </c>
       <c r="F28" s="4"/>
-      <c r="G28" s="1"/>
       <c r="H28" s="4"/>
       <c r="I28" s="1" t="s">
         <v>78</v>
@@ -2224,10 +2221,10 @@
         <v>44</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>138</v>
-      </c>
-      <c r="G29" s="33" t="s">
         <v>137</v>
+      </c>
+      <c r="G29" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="H29" s="35" t="s">
         <v>119</v>
@@ -2249,10 +2246,10 @@
         <v>45</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>139</v>
-      </c>
-      <c r="G30" s="33" t="s">
-        <v>137</v>
+        <v>138</v>
+      </c>
+      <c r="G30" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="H30" s="35"/>
       <c r="I30" s="33" t="s">
@@ -2269,12 +2266,12 @@
         <v>43</v>
       </c>
       <c r="E31" s="37" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F31" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="G31" s="33"/>
+        <v>139</v>
+      </c>
+      <c r="G31" s="40"/>
       <c r="H31" s="35" t="s">
         <v>46</v>
       </c>
@@ -2295,7 +2292,7 @@
         <v>52</v>
       </c>
       <c r="F32" s="9"/>
-      <c r="G32" s="8"/>
+      <c r="G32" s="41"/>
       <c r="H32" s="9"/>
       <c r="I32" s="8" t="s">
         <v>78</v>
@@ -2314,7 +2311,7 @@
         <v>51</v>
       </c>
       <c r="F33" s="13"/>
-      <c r="G33" s="12"/>
+      <c r="G33" s="42"/>
       <c r="H33" s="13" t="s">
         <v>120</v>
       </c>
@@ -2335,9 +2332,9 @@
         <v>53</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>140</v>
-      </c>
-      <c r="G34" s="33"/>
+        <v>139</v>
+      </c>
+      <c r="G34" s="40"/>
       <c r="H34" s="35"/>
       <c r="I34" s="33" t="s">
         <v>112</v>
@@ -2356,7 +2353,7 @@
         <v>54</v>
       </c>
       <c r="F35" s="6"/>
-      <c r="G35" s="5"/>
+      <c r="G35" s="43"/>
       <c r="H35" s="6" t="s">
         <v>121</v>
       </c>
@@ -2377,7 +2374,7 @@
         <v>55</v>
       </c>
       <c r="F36" s="9"/>
-      <c r="G36" s="8"/>
+      <c r="G36" s="41"/>
       <c r="H36" s="9" t="s">
         <v>122</v>
       </c>
@@ -2398,7 +2395,7 @@
         <v>56</v>
       </c>
       <c r="F37" s="6"/>
-      <c r="G37" s="5"/>
+      <c r="G37" s="43"/>
       <c r="H37" s="6"/>
       <c r="I37" s="5" t="s">
         <v>78</v>
@@ -2417,9 +2414,9 @@
         <v>57</v>
       </c>
       <c r="F38" s="13"/>
-      <c r="G38" s="12"/>
+      <c r="G38" s="42"/>
       <c r="H38" s="13" t="s">
-        <v>123</v>
+        <v>147</v>
       </c>
       <c r="I38" s="12" t="s">
         <v>78</v>
@@ -2438,13 +2435,13 @@
         <v>59</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="G39" s="33" t="s">
-        <v>137</v>
+        <v>140</v>
+      </c>
+      <c r="G39" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="H39" s="35" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I39" s="33" t="s">
         <v>112</v>
@@ -2463,13 +2460,13 @@
         <v>61</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="G40" s="33" t="s">
-        <v>137</v>
+        <v>141</v>
+      </c>
+      <c r="G40" s="40" t="s">
+        <v>136</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I40" s="33" t="s">
         <v>112</v>
@@ -2488,9 +2485,9 @@
         <v>64</v>
       </c>
       <c r="F41" s="6"/>
-      <c r="G41" s="5"/>
+      <c r="G41" s="43"/>
       <c r="H41" s="6" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>78</v>
@@ -2509,51 +2506,58 @@
         <v>65</v>
       </c>
       <c r="F42" s="4"/>
-      <c r="G42" s="1"/>
       <c r="H42" s="4"/>
       <c r="I42" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="10" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A43" s="17" t="s">
+    <row r="43" spans="1:9" s="36" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A43" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8" t="s">
+      <c r="B43" s="33"/>
+      <c r="C43" s="33"/>
+      <c r="D43" s="33" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="23" t="s">
+      <c r="E43" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="9"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="9" t="s">
+      <c r="F43" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="G43" s="33" t="s">
+        <v>136</v>
+      </c>
+      <c r="H43" s="35" t="s">
+        <v>126</v>
+      </c>
+      <c r="I43" s="33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" s="36" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="B44" s="33"/>
+      <c r="C44" s="33"/>
+      <c r="D44" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="E44" s="37" t="s">
+        <v>68</v>
+      </c>
+      <c r="F44" s="35" t="s">
+        <v>145</v>
+      </c>
+      <c r="G44" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="H44" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="I43" s="8" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="44" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="16" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="5"/>
-      <c r="C44" s="5"/>
-      <c r="D44" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="E44" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="F44" s="6"/>
-      <c r="G44" s="5"/>
-      <c r="H44" s="6" t="s">
-        <v>128</v>
-      </c>
-      <c r="I44" s="5" t="s">
+      <c r="I44" s="33" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2570,7 +2574,7 @@
         <v>70</v>
       </c>
       <c r="F45" s="9"/>
-      <c r="G45" s="8"/>
+      <c r="G45" s="41"/>
       <c r="H45" s="11" t="s">
         <v>71</v>
       </c>
@@ -2578,24 +2582,28 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="10" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A46" s="17" t="s">
+    <row r="46" spans="1:9" s="36" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A46" s="32" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8" t="s">
+      <c r="B46" s="33"/>
+      <c r="C46" s="33"/>
+      <c r="D46" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E46" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="F46" s="9"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="9" t="s">
-        <v>129</v>
-      </c>
-      <c r="I46" s="8" t="s">
+      <c r="F46" s="40" t="s">
+        <v>146</v>
+      </c>
+      <c r="G46" s="40" t="s">
+        <v>136</v>
+      </c>
+      <c r="H46" s="35" t="s">
+        <v>128</v>
+      </c>
+      <c r="I46" s="33" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2611,7 +2619,6 @@
       <c r="E47" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="G47" s="2"/>
       <c r="I47" s="1" t="s">
         <v>78</v>
       </c>
@@ -2628,7 +2635,6 @@
       <c r="E48" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="G48" s="2"/>
       <c r="I48" s="1" t="s">
         <v>78</v>
       </c>
@@ -2645,7 +2651,6 @@
       <c r="E49" s="29" t="s">
         <v>80</v>
       </c>
-      <c r="G49" s="2"/>
       <c r="I49" s="1" t="s">
         <v>78</v>
       </c>
@@ -2662,7 +2667,6 @@
       <c r="E50" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="G50" s="2"/>
       <c r="I50" s="1" t="s">
         <v>78</v>
       </c>
@@ -2679,7 +2683,6 @@
       <c r="E51" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="G51" s="2"/>
       <c r="I51" s="1" t="s">
         <v>78</v>
       </c>
@@ -2698,7 +2701,6 @@
       <c r="E52" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="G52" s="2"/>
       <c r="I52" s="1" t="s">
         <v>78</v>
       </c>
@@ -2717,7 +2719,6 @@
       <c r="E53" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="G53" s="2"/>
       <c r="I53" s="1" t="s">
         <v>78</v>
       </c>
@@ -2736,7 +2737,6 @@
       <c r="E54" s="29" t="s">
         <v>90</v>
       </c>
-      <c r="G54" s="2"/>
       <c r="I54" s="1" t="s">
         <v>78</v>
       </c>
@@ -2753,7 +2753,6 @@
       <c r="E55" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="G55" s="2"/>
       <c r="I55" s="1" t="s">
         <v>78</v>
       </c>
@@ -2770,7 +2769,6 @@
       <c r="E56" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="G56" s="2"/>
       <c r="I56" s="1" t="s">
         <v>78</v>
       </c>
@@ -2787,7 +2785,6 @@
       <c r="E57" s="29" t="s">
         <v>94</v>
       </c>
-      <c r="G57" s="2"/>
       <c r="I57" s="1" t="s">
         <v>78</v>
       </c>
@@ -2809,7 +2806,6 @@
       <c r="F58" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="G58" s="2"/>
       <c r="I58" s="1" t="s">
         <v>78</v>
       </c>
@@ -2828,7 +2824,6 @@
       <c r="E59" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="G59" s="2"/>
       <c r="I59" s="1" t="s">
         <v>78</v>
       </c>
@@ -2847,7 +2842,6 @@
       <c r="E60" s="29" t="s">
         <v>102</v>
       </c>
-      <c r="G60" s="2"/>
       <c r="I60" s="1" t="s">
         <v>78</v>
       </c>
@@ -2866,7 +2860,6 @@
       <c r="E61" s="29" t="s">
         <v>104</v>
       </c>
-      <c r="G61" s="2"/>
       <c r="I61" s="1" t="s">
         <v>78</v>
       </c>
@@ -2885,7 +2878,6 @@
       <c r="E62" s="29" t="s">
         <v>106</v>
       </c>
-      <c r="G62" s="2"/>
       <c r="I62" s="1" t="s">
         <v>78</v>
       </c>
@@ -2904,7 +2896,6 @@
       <c r="E63" s="29" t="s">
         <v>107</v>
       </c>
-      <c r="G63" s="2"/>
       <c r="I63" s="1" t="s">
         <v>78</v>
       </c>
@@ -2923,7 +2914,6 @@
       <c r="E64" s="29" t="s">
         <v>111</v>
       </c>
-      <c r="G64" s="2"/>
       <c r="I64" s="1" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
Update spreadsheet of actions.
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A6EAF25-B742-D54B-ADB1-FC89240CF071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17607BAE-B32E-FE4A-B636-EEF6EA51B015}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="36900" windowHeight="28040" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
@@ -1637,8 +1637,8 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H39" sqref="H39"/>
+      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A73" sqref="A73:XFD73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Editing the methods section.
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA834BC3-B937-6A4A-B953-3A19CA853E0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6B9098-2C10-B646-8429-4C8CB96DC33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="36900" windowHeight="28040" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="152">
   <si>
     <t>Commenter</t>
   </si>
@@ -768,6 +768,21 @@
   </si>
   <si>
     <t>Fix the misspelling</t>
+  </si>
+  <si>
+    <t>Yes. Laura is right. I made a small change to make this clearer</t>
+  </si>
+  <si>
+    <t>Didn't quite make this change, but did something better. Material exergy is defined as the maximum amount of work
+that could be extracted
+by an ideal, reversible process
+that brings the mixture of materials
+into equilibrium with the reference environment,
+characterized by
+particle size ($d_0$),
+temperature ($T_0$),
+pressure ($P_0$), and
+chemical composition ($y_{i,0}$).</t>
   </si>
 </sst>
 </file>
@@ -1669,7 +1684,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1844,40 +1859,50 @@
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="15" t="s">
+    <row r="8" spans="1:9" s="36" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1" t="s">
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
+      <c r="F8" s="35" t="s">
+        <v>150</v>
+      </c>
+      <c r="G8" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="H8" s="35"/>
+      <c r="I8" s="33" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" s="36" customFormat="1" ht="176" x14ac:dyDescent="0.2">
+      <c r="A9" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1">
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33">
         <v>218</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="38" t="s">
         <v>129</v>
       </c>
-      <c r="F9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="1" t="s">
-        <v>78</v>
+      <c r="F9" s="35" t="s">
+        <v>151</v>
+      </c>
+      <c r="G9" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="H9" s="35"/>
+      <c r="I9" s="33" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update chemical exergy section.
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F6B9098-2C10-B646-8429-4C8CB96DC33E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7A6774-75DB-AC47-A4D1-A4598217D2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="36900" windowHeight="28040" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Review 1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="153">
   <si>
     <t>Commenter</t>
   </si>
@@ -783,6 +783,9 @@
 temperature ($T_0$),
 pressure ($P_0$), and
 chemical composition ($y_{i,0}$).</t>
+  </si>
+  <si>
+    <t>Adjusted the wording a little</t>
   </si>
 </sst>
 </file>
@@ -1684,7 +1687,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E10" sqref="E10"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1800,22 +1803,27 @@
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
+    <row r="5" spans="1:9" s="49" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1">
+      <c r="B5" s="45"/>
+      <c r="C5" s="45"/>
+      <c r="D5" s="45">
         <v>74</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="46" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="1" t="s">
-        <v>78</v>
+      <c r="F5" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="G5" s="48" t="s">
+        <v>135</v>
+      </c>
+      <c r="H5" s="47"/>
+      <c r="I5" s="45" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Working on Laura's comments.
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B7A6774-75DB-AC47-A4D1-A4598217D2C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C804501B-FDC4-7E46-AE2A-EC13EEF94EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="159">
   <si>
     <t>Commenter</t>
   </si>
@@ -408,9 +408,6 @@
   </si>
   <si>
     <t>Rephrase caption to address the comment.</t>
-  </si>
-  <si>
-    <t>Put **** in the text to indicate that we will figure out the locations when the SI is ocmplete.</t>
   </si>
   <si>
     <t>Use matrix subtraction instead of equation.</t>
@@ -786,6 +783,27 @@
   </si>
   <si>
     <t>Adjusted the wording a little</t>
+  </si>
+  <si>
+    <t>I disagree with this suggestion. I think it is fine to wait until later to provide details of the location for pig iron production (South Afric).</t>
+  </si>
+  <si>
+    <t>No changes made.</t>
+  </si>
+  <si>
+    <t>Singnficantly revised the methods section for consistency.</t>
+  </si>
+  <si>
+    <t>Added **** in the text to indicate that we will figure out the locations when the SI is ocmplete.</t>
+  </si>
+  <si>
+    <t>This comment is unclear.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I disagree. I think the detailed description is good. </t>
+  </si>
+  <si>
+    <t>Added more to the legend.</t>
   </si>
 </sst>
 </file>
@@ -927,7 +945,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1068,6 +1086,9 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1686,8 +1707,8 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1743,10 +1764,10 @@
         <v>10</v>
       </c>
       <c r="F2" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G2" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H2" s="35" t="s">
         <v>113</v>
@@ -1766,13 +1787,13 @@
         <v>12</v>
       </c>
       <c r="F3" s="50" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G3" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="I3" s="33" t="s">
         <v>112</v>
@@ -1791,10 +1812,10 @@
         <v>13</v>
       </c>
       <c r="F4" s="35" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H4" s="35" t="s">
         <v>113</v>
@@ -1816,32 +1837,39 @@
         <v>14</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G5" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H5" s="47"/>
       <c r="I5" s="45" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="15" t="s">
+    <row r="6" spans="1:9" s="49" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1">
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45">
         <v>151</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="46" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="1" t="s">
-        <v>78</v>
+      <c r="F6" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G6" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="47" t="s">
+        <v>152</v>
+      </c>
+      <c r="I6" s="45" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="49" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1854,13 +1882,13 @@
         <v>159</v>
       </c>
       <c r="E7" s="46" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G7" s="48" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H7" s="47"/>
       <c r="I7" s="45" t="s">
@@ -1880,10 +1908,10 @@
         <v>17</v>
       </c>
       <c r="F8" s="35" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G8" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H8" s="35"/>
       <c r="I8" s="33" t="s">
@@ -1900,35 +1928,40 @@
         <v>218</v>
       </c>
       <c r="E9" s="38" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F9" s="35" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G9" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H9" s="35"/>
       <c r="I9" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="15" t="s">
+    <row r="10" spans="1:9" s="49" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1" t="s">
+      <c r="B10" s="45"/>
+      <c r="C10" s="45"/>
+      <c r="D10" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="E10" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="1" t="s">
-        <v>78</v>
+      <c r="F10" s="47" t="s">
+        <v>154</v>
+      </c>
+      <c r="G10" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" s="47"/>
+      <c r="I10" s="45" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:9" s="36" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -1944,10 +1977,10 @@
         <v>20</v>
       </c>
       <c r="F11" s="35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G11" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H11" s="35" t="s">
         <v>114</v>
@@ -1966,134 +1999,159 @@
         <v>21</v>
       </c>
       <c r="E12" s="38" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F12" s="35" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G12" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H12" s="35"/>
       <c r="I12" s="33" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+    <row r="13" spans="1:9" s="49" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1" t="s">
+      <c r="B13" s="45"/>
+      <c r="C13" s="45"/>
+      <c r="D13" s="45" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="4"/>
-      <c r="H13" s="4" t="s">
+      <c r="F13" s="47" t="s">
+        <v>155</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="51"/>
+      <c r="I13" s="45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" s="49" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45">
+        <v>438</v>
+      </c>
+      <c r="E14" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="F14" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G14" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="47" t="s">
+        <v>156</v>
+      </c>
+      <c r="I14" s="45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="49" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="45"/>
+      <c r="C15" s="45"/>
+      <c r="D15" s="45" t="s">
+        <v>26</v>
+      </c>
+      <c r="E15" s="46" t="s">
+        <v>25</v>
+      </c>
+      <c r="F15" s="47" t="s">
+        <v>153</v>
+      </c>
+      <c r="G15" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="47" t="s">
+        <v>157</v>
+      </c>
+      <c r="I15" s="45" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" s="49" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="44" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="45"/>
+      <c r="C16" s="45"/>
+      <c r="D16" s="45" t="s">
+        <v>27</v>
+      </c>
+      <c r="E16" s="46" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" s="47" t="s">
+        <v>143</v>
+      </c>
+      <c r="G16" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" s="47" t="s">
         <v>115</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
+      <c r="I16" s="45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" s="49" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1">
-        <v>438</v>
-      </c>
-      <c r="E14" s="21" t="s">
-        <v>24</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="H14" s="4"/>
-      <c r="I14" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" ht="85" x14ac:dyDescent="0.2">
-      <c r="A15" s="15" t="s">
+      <c r="B17" s="45"/>
+      <c r="C17" s="45"/>
+      <c r="D17" s="45">
+        <v>487</v>
+      </c>
+      <c r="E17" s="46" t="s">
+        <v>29</v>
+      </c>
+      <c r="F17" s="47"/>
+      <c r="G17" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="47"/>
+      <c r="I17" s="45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" s="49" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E15" s="21" t="s">
-        <v>25</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" s="36" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B16" s="33"/>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33" t="s">
-        <v>27</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F16" s="35" t="s">
-        <v>144</v>
-      </c>
-      <c r="G16" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>116</v>
-      </c>
-      <c r="I16" s="33" t="s">
+      <c r="B18" s="45"/>
+      <c r="C18" s="45"/>
+      <c r="D18" s="45" t="s">
+        <v>30</v>
+      </c>
+      <c r="E18" s="46" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="47"/>
+      <c r="G18" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="47" t="s">
+        <v>158</v>
+      </c>
+      <c r="I18" s="45" t="s">
         <v>112</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1">
-        <v>487</v>
-      </c>
-      <c r="E17" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="1" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="68" x14ac:dyDescent="0.2">
@@ -2110,7 +2168,7 @@
       </c>
       <c r="F19" s="4"/>
       <c r="H19" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>78</v>
@@ -2162,7 +2220,7 @@
         <v>35</v>
       </c>
       <c r="E22" s="21" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F22" s="4"/>
       <c r="H22" s="4"/>
@@ -2202,7 +2260,7 @@
       </c>
       <c r="F24" s="4"/>
       <c r="H24" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I24" s="1" t="s">
         <v>78</v>
@@ -2218,7 +2276,7 @@
         <v>37</v>
       </c>
       <c r="E25" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F25" s="4"/>
       <c r="H25" s="4"/>
@@ -2254,7 +2312,7 @@
         <v>718</v>
       </c>
       <c r="E27" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F27" s="4"/>
       <c r="H27" s="4"/>
@@ -2293,13 +2351,13 @@
         <v>44</v>
       </c>
       <c r="F29" s="35" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G29" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H29" s="35" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="I29" s="33" t="s">
         <v>112</v>
@@ -2318,10 +2376,10 @@
         <v>45</v>
       </c>
       <c r="F30" s="35" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G30" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H30" s="35"/>
       <c r="I30" s="33" t="s">
@@ -2338,10 +2396,10 @@
         <v>43</v>
       </c>
       <c r="E31" s="37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="F31" s="35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G31" s="40"/>
       <c r="H31" s="35" t="s">
@@ -2385,7 +2443,7 @@
       <c r="F33" s="13"/>
       <c r="G33" s="42"/>
       <c r="H33" s="13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I33" s="12" t="s">
         <v>78</v>
@@ -2404,7 +2462,7 @@
         <v>53</v>
       </c>
       <c r="F34" s="35" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G34" s="40"/>
       <c r="H34" s="35"/>
@@ -2427,7 +2485,7 @@
       <c r="F35" s="6"/>
       <c r="G35" s="43"/>
       <c r="H35" s="6" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I35" s="5" t="s">
         <v>78</v>
@@ -2448,7 +2506,7 @@
       <c r="F36" s="9"/>
       <c r="G36" s="41"/>
       <c r="H36" s="9" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>78</v>
@@ -2488,7 +2546,7 @@
       <c r="F38" s="13"/>
       <c r="G38" s="42"/>
       <c r="H38" s="13" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I38" s="12" t="s">
         <v>78</v>
@@ -2507,13 +2565,13 @@
         <v>59</v>
       </c>
       <c r="F39" s="35" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G39" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H39" s="35" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="I39" s="33" t="s">
         <v>112</v>
@@ -2532,13 +2590,13 @@
         <v>61</v>
       </c>
       <c r="F40" s="35" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G40" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="I40" s="33" t="s">
         <v>112</v>
@@ -2559,7 +2617,7 @@
       <c r="F41" s="6"/>
       <c r="G41" s="43"/>
       <c r="H41" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="I41" s="5" t="s">
         <v>78</v>
@@ -2596,13 +2654,13 @@
         <v>66</v>
       </c>
       <c r="F43" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G43" s="33" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="I43" s="33" t="s">
         <v>112</v>
@@ -2621,13 +2679,13 @@
         <v>68</v>
       </c>
       <c r="F44" s="35" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G44" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H44" s="35" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="I44" s="33" t="s">
         <v>112</v>
@@ -2667,13 +2725,13 @@
         <v>73</v>
       </c>
       <c r="F46" s="40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G46" s="40" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H46" s="35" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="I46" s="33" t="s">
         <v>112</v>

</xml_diff>

<commit_message>
Working on heat loss idea.
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C804501B-FDC4-7E46-AE2A-EC13EEF94EFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{035AA3C0-4C8C-6E44-B111-76EF38533EFB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="162">
   <si>
     <t>Commenter</t>
   </si>
@@ -804,6 +804,15 @@
   </si>
   <si>
     <t>Added more to the legend.</t>
+  </si>
+  <si>
+    <t>Changed to "desired".</t>
+  </si>
+  <si>
+    <t>. --&gt; ,</t>
+  </si>
+  <si>
+    <t>Deleted one</t>
   </si>
 </sst>
 </file>
@@ -1707,8 +1716,8 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
+      <pane ySplit="1" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2154,60 +2163,75 @@
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" s="15" t="s">
+    <row r="19" spans="1:9" s="49" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1">
+      <c r="B19" s="45"/>
+      <c r="C19" s="45"/>
+      <c r="D19" s="45">
         <v>526</v>
       </c>
-      <c r="E19" s="21" t="s">
+      <c r="E19" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="4"/>
-      <c r="H19" s="4" t="s">
+      <c r="F19" s="47" t="s">
+        <v>159</v>
+      </c>
+      <c r="G19" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="47" t="s">
         <v>116</v>
       </c>
-      <c r="I19" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="15" t="s">
+      <c r="I19" s="45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" s="49" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1">
+      <c r="B20" s="45"/>
+      <c r="C20" s="45"/>
+      <c r="D20" s="45">
         <v>527</v>
       </c>
-      <c r="E20" s="21" t="s">
+      <c r="E20" s="46" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="15" t="s">
+      <c r="F20" s="47" t="s">
+        <v>160</v>
+      </c>
+      <c r="G20" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="47"/>
+      <c r="I20" s="45" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" s="49" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="44" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1">
+      <c r="B21" s="45"/>
+      <c r="C21" s="45"/>
+      <c r="D21" s="45">
         <v>533</v>
       </c>
-      <c r="E21" s="21" t="s">
+      <c r="E21" s="46" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="1" t="s">
-        <v>78</v>
+      <c r="F21" s="47" t="s">
+        <v>161</v>
+      </c>
+      <c r="G21" s="48" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="47"/>
+      <c r="I21" s="45" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="53" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Update Excel sheet punch list
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2685BD39-028D-7346-AB9D-9FE3F668BFD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3381750D-2DB6-5B44-9AAA-B3B4FBE47D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="169">
   <si>
     <t>Commenter</t>
   </si>
@@ -831,6 +831,9 @@
   </si>
   <si>
     <t>We decided to go with a negative value and Figure 1 (Tania's diagram).</t>
+  </si>
+  <si>
+    <t>Added in chemical exergy section.</t>
   </si>
 </sst>
 </file>
@@ -1031,9 +1034,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1110,6 +1110,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1728,19 +1731,19 @@
   <dimension ref="A1:I64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E48" sqref="E48"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17.6640625" style="19" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.1640625" style="28" customWidth="1"/>
+    <col min="5" max="5" width="61.1640625" style="27" customWidth="1"/>
     <col min="6" max="6" width="48.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="36.1640625" style="37" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" style="36" customWidth="1"/>
     <col min="8" max="8" width="66.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="29"/>
+    <col min="9" max="9" width="8.83203125" style="28"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
@@ -1762,7 +1765,7 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="G1" s="36" t="s">
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
@@ -1772,477 +1775,477 @@
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="34" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:9" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="31"/>
-      <c r="C2" s="31"/>
-      <c r="D2" s="31" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="30"/>
+      <c r="D2" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="36" t="s">
+      <c r="E2" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="33" t="s">
+      <c r="F2" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H2" s="33" t="s">
+      <c r="G2" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="31" t="s">
+      <c r="I2" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="31" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:9" s="30" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="31" t="s">
+      <c r="E3" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="48" t="s">
+      <c r="F3" s="47" t="s">
         <v>147</v>
       </c>
-      <c r="G3" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" s="33" t="s">
+      <c r="G3" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="32" t="s">
         <v>146</v>
       </c>
-      <c r="I3" s="31" t="s">
+      <c r="I3" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="34" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:9" s="33" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31">
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30">
         <v>48</v>
       </c>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="32" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" s="33" t="s">
+      <c r="G4" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="32" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="31" t="s">
+      <c r="I4" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="47" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
+    <row r="5" spans="1:9" s="46" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="43"/>
-      <c r="C5" s="43"/>
-      <c r="D5" s="43">
+      <c r="B5" s="42"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42">
         <v>74</v>
       </c>
-      <c r="E5" s="44" t="s">
+      <c r="E5" s="43" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="45" t="s">
+      <c r="F5" s="44" t="s">
         <v>151</v>
       </c>
-      <c r="G5" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="45"/>
-      <c r="I5" s="43" t="s">
+      <c r="G5" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="44"/>
+      <c r="I5" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="47" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
+    <row r="6" spans="1:9" s="46" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="43"/>
-      <c r="C6" s="43"/>
-      <c r="D6" s="43">
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42">
         <v>151</v>
       </c>
-      <c r="E6" s="44" t="s">
+      <c r="E6" s="43" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="45" t="s">
+      <c r="F6" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="G6" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H6" s="45" t="s">
+      <c r="G6" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="44" t="s">
         <v>152</v>
       </c>
-      <c r="I6" s="43" t="s">
+      <c r="I6" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="42" t="s">
+    <row r="7" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="43"/>
-      <c r="C7" s="43"/>
-      <c r="D7" s="43">
+      <c r="B7" s="42"/>
+      <c r="C7" s="42"/>
+      <c r="D7" s="42">
         <v>159</v>
       </c>
-      <c r="E7" s="44" t="s">
+      <c r="E7" s="43" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="45" t="s">
+      <c r="F7" s="44" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H7" s="45"/>
-      <c r="I7" s="43" t="s">
+      <c r="G7" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="44"/>
+      <c r="I7" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="34" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:9" s="33" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="31"/>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31" t="s">
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="36" t="s">
+      <c r="E8" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="33" t="s">
+      <c r="F8" s="32" t="s">
         <v>149</v>
       </c>
-      <c r="G8" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H8" s="33"/>
-      <c r="I8" s="31" t="s">
+      <c r="G8" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" s="32"/>
+      <c r="I8" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="34" customFormat="1" ht="176" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
+    <row r="9" spans="1:9" s="33" customFormat="1" ht="176" x14ac:dyDescent="0.2">
+      <c r="A9" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="31"/>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30">
         <v>218</v>
       </c>
-      <c r="E9" s="36" t="s">
+      <c r="E9" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="F9" s="33" t="s">
+      <c r="F9" s="32" t="s">
         <v>150</v>
       </c>
-      <c r="G9" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H9" s="33"/>
-      <c r="I9" s="31" t="s">
+      <c r="G9" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H9" s="32"/>
+      <c r="I9" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="47" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
+    <row r="10" spans="1:9" s="46" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="43"/>
-      <c r="C10" s="43"/>
-      <c r="D10" s="43" t="s">
+      <c r="B10" s="42"/>
+      <c r="C10" s="42"/>
+      <c r="D10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="44" t="s">
+      <c r="E10" s="43" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="45" t="s">
+      <c r="F10" s="44" t="s">
         <v>154</v>
       </c>
-      <c r="G10" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" s="45"/>
-      <c r="I10" s="43" t="s">
+      <c r="G10" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" s="44"/>
+      <c r="I10" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="34" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="30" t="s">
+    <row r="11" spans="1:9" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="31"/>
-      <c r="C11" s="31"/>
-      <c r="D11" s="31" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="33" t="s">
+      <c r="F11" s="32" t="s">
         <v>141</v>
       </c>
-      <c r="G11" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" s="33" t="s">
+      <c r="G11" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="34" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+    <row r="12" spans="1:9" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="31"/>
-      <c r="C12" s="31"/>
-      <c r="D12" s="31" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="F12" s="33" t="s">
+      <c r="F12" s="32" t="s">
         <v>142</v>
       </c>
-      <c r="G12" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H12" s="33"/>
-      <c r="I12" s="31" t="s">
+      <c r="G12" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" s="32"/>
+      <c r="I12" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="47" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="42" t="s">
+    <row r="13" spans="1:9" s="46" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="43"/>
-      <c r="C13" s="43"/>
-      <c r="D13" s="43" t="s">
+      <c r="B13" s="42"/>
+      <c r="C13" s="42"/>
+      <c r="D13" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="44" t="s">
+      <c r="E13" s="43" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="45" t="s">
+      <c r="F13" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="G13" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H13" s="49"/>
-      <c r="I13" s="43" t="s">
+      <c r="G13" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="48"/>
+      <c r="I13" s="42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
+    <row r="14" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="43"/>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43">
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
+      <c r="D14" s="42">
         <v>438</v>
       </c>
-      <c r="E14" s="44" t="s">
+      <c r="E14" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="45" t="s">
+      <c r="F14" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="G14" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H14" s="45" t="s">
+      <c r="G14" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="I14" s="43" t="s">
+      <c r="I14" s="42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="47" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A15" s="42" t="s">
+    <row r="15" spans="1:9" s="46" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="43"/>
-      <c r="C15" s="43"/>
-      <c r="D15" s="43" t="s">
+      <c r="B15" s="42"/>
+      <c r="C15" s="42"/>
+      <c r="D15" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="44" t="s">
+      <c r="E15" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="45" t="s">
+      <c r="F15" s="44" t="s">
         <v>153</v>
       </c>
-      <c r="G15" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H15" s="45" t="s">
+      <c r="G15" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="I15" s="43" t="s">
+      <c r="I15" s="42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="47" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="42" t="s">
+    <row r="16" spans="1:9" s="46" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="43"/>
-      <c r="C16" s="43"/>
-      <c r="D16" s="43" t="s">
+      <c r="B16" s="42"/>
+      <c r="C16" s="42"/>
+      <c r="D16" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="44" t="s">
+      <c r="E16" s="43" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="45" t="s">
+      <c r="F16" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="G16" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H16" s="45" t="s">
+      <c r="G16" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="I16" s="43" t="s">
+      <c r="I16" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="42" t="s">
+    <row r="17" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="43"/>
-      <c r="C17" s="43"/>
-      <c r="D17" s="43">
+      <c r="B17" s="42"/>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42">
         <v>487</v>
       </c>
-      <c r="E17" s="44" t="s">
+      <c r="E17" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="45"/>
-      <c r="G17" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H17" s="45"/>
-      <c r="I17" s="43" t="s">
+      <c r="F17" s="44"/>
+      <c r="G17" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="44"/>
+      <c r="I17" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="47" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
+    <row r="18" spans="1:9" s="46" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="43"/>
-      <c r="C18" s="43"/>
-      <c r="D18" s="43" t="s">
+      <c r="B18" s="42"/>
+      <c r="C18" s="42"/>
+      <c r="D18" s="42" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="44" t="s">
+      <c r="E18" s="43" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="45"/>
-      <c r="G18" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H18" s="45" t="s">
+      <c r="F18" s="44"/>
+      <c r="G18" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="44" t="s">
         <v>158</v>
       </c>
-      <c r="I18" s="43" t="s">
+      <c r="I18" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="47" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" s="42" t="s">
+    <row r="19" spans="1:9" s="46" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="43"/>
-      <c r="C19" s="43"/>
-      <c r="D19" s="43">
+      <c r="B19" s="42"/>
+      <c r="C19" s="42"/>
+      <c r="D19" s="42">
         <v>526</v>
       </c>
-      <c r="E19" s="44" t="s">
+      <c r="E19" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="45" t="s">
+      <c r="F19" s="44" t="s">
         <v>159</v>
       </c>
-      <c r="G19" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H19" s="45" t="s">
+      <c r="G19" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="I19" s="43" t="s">
+      <c r="I19" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="42" t="s">
+    <row r="20" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="43"/>
-      <c r="C20" s="43"/>
-      <c r="D20" s="43">
+      <c r="B20" s="42"/>
+      <c r="C20" s="42"/>
+      <c r="D20" s="42">
         <v>527</v>
       </c>
-      <c r="E20" s="44" t="s">
+      <c r="E20" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="45" t="s">
+      <c r="F20" s="44" t="s">
         <v>160</v>
       </c>
-      <c r="G20" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H20" s="45"/>
-      <c r="I20" s="43" t="s">
+      <c r="G20" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="44"/>
+      <c r="I20" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="42" t="s">
+    <row r="21" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="43"/>
-      <c r="C21" s="43"/>
-      <c r="D21" s="43">
+      <c r="B21" s="42"/>
+      <c r="C21" s="42"/>
+      <c r="D21" s="42">
         <v>533</v>
       </c>
-      <c r="E21" s="44" t="s">
+      <c r="E21" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="45" t="s">
+      <c r="F21" s="44" t="s">
         <v>161</v>
       </c>
-      <c r="G21" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H21" s="45"/>
-      <c r="I21" s="43" t="s">
+      <c r="G21" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="44"/>
+      <c r="I21" s="42" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2282,28 +2285,28 @@
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="42" t="s">
+    <row r="24" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="43"/>
-      <c r="C24" s="43"/>
-      <c r="D24" s="43" t="s">
+      <c r="B24" s="42"/>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="E24" s="43" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="45" t="s">
+      <c r="F24" s="44" t="s">
         <v>162</v>
       </c>
-      <c r="G24" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H24" s="45" t="s">
+      <c r="G24" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H24" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="I24" s="43" t="s">
+      <c r="I24" s="42" t="s">
         <v>78</v>
       </c>
     </row>
@@ -2325,47 +2328,47 @@
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="42" t="s">
+    <row r="26" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="43"/>
-      <c r="C26" s="43"/>
-      <c r="D26" s="43">
+      <c r="B26" s="42"/>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42">
         <v>697</v>
       </c>
-      <c r="E26" s="44" t="s">
+      <c r="E26" s="43" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="45" t="s">
+      <c r="F26" s="44" t="s">
         <v>163</v>
       </c>
-      <c r="G26" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H26" s="45"/>
-      <c r="I26" s="43" t="s">
+      <c r="G26" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="44"/>
+      <c r="I26" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="47" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="42" t="s">
+    <row r="27" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43">
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42">
         <v>718</v>
       </c>
-      <c r="E27" s="44" t="s">
+      <c r="E27" s="43" t="s">
         <v>132</v>
       </c>
-      <c r="F27" s="45" t="s">
+      <c r="F27" s="44" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="46"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="43" t="s">
+      <c r="G27" s="45"/>
+      <c r="H27" s="44"/>
+      <c r="I27" s="42" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2387,97 +2390,97 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="34" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" s="30" t="s">
+    <row r="29" spans="1:9" s="33" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="31"/>
-      <c r="D29" s="31">
+      <c r="B29" s="30"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30">
         <v>18</v>
       </c>
-      <c r="E29" s="32" t="s">
+      <c r="E29" s="31" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="33" t="s">
+      <c r="F29" s="32" t="s">
         <v>135</v>
       </c>
-      <c r="G29" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H29" s="33" t="s">
+      <c r="G29" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H29" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="I29" s="31" t="s">
+      <c r="I29" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="34" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A30" s="30" t="s">
+    <row r="30" spans="1:9" s="33" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A30" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="31">
+      <c r="B30" s="30"/>
+      <c r="C30" s="30"/>
+      <c r="D30" s="30">
         <v>51</v>
       </c>
-      <c r="E30" s="35" t="s">
+      <c r="E30" s="34" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="33" t="s">
+      <c r="F30" s="32" t="s">
         <v>136</v>
       </c>
-      <c r="G30" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H30" s="33"/>
-      <c r="I30" s="31" t="s">
+      <c r="G30" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H30" s="32"/>
+      <c r="I30" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="34" customFormat="1" ht="144" x14ac:dyDescent="0.2">
-      <c r="A31" s="30" t="s">
+    <row r="31" spans="1:9" s="33" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+      <c r="A31" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="31"/>
-      <c r="D31" s="31" t="s">
+      <c r="B31" s="30"/>
+      <c r="C31" s="30"/>
+      <c r="D31" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="33" t="s">
+      <c r="F31" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="G31" s="38"/>
-      <c r="H31" s="33" t="s">
+      <c r="G31" s="37"/>
+      <c r="H31" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="31" t="s">
+      <c r="I31" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="47" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="42" t="s">
+    <row r="32" spans="1:9" s="46" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="43"/>
-      <c r="C32" s="43"/>
-      <c r="D32" s="43">
+      <c r="B32" s="42"/>
+      <c r="C32" s="42"/>
+      <c r="D32" s="42">
         <v>74</v>
       </c>
-      <c r="E32" s="44" t="s">
+      <c r="E32" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="F32" s="45" t="s">
+      <c r="F32" s="44" t="s">
         <v>165</v>
       </c>
-      <c r="G32" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H32" s="45"/>
-      <c r="I32" s="43" t="s">
+      <c r="G32" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H32" s="44"/>
+      <c r="I32" s="42" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2490,11 +2493,11 @@
       <c r="D33" s="12" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="24" t="s">
+      <c r="E33" s="23" t="s">
         <v>51</v>
       </c>
       <c r="F33" s="13"/>
-      <c r="G33" s="40"/>
+      <c r="G33" s="39"/>
       <c r="H33" s="13" t="s">
         <v>118</v>
       </c>
@@ -2502,24 +2505,24 @@
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="34" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A34" s="30" t="s">
+    <row r="34" spans="1:9" s="33" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A34" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="31"/>
-      <c r="C34" s="31"/>
-      <c r="D34" s="31" t="s">
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="33" t="s">
+      <c r="F34" s="32" t="s">
         <v>137</v>
       </c>
-      <c r="G34" s="38"/>
-      <c r="H34" s="33"/>
-      <c r="I34" s="31" t="s">
+      <c r="G34" s="37"/>
+      <c r="H34" s="32"/>
+      <c r="I34" s="30" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2532,11 +2535,11 @@
       <c r="D35" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="25" t="s">
+      <c r="E35" s="24" t="s">
         <v>54</v>
       </c>
       <c r="F35" s="6"/>
-      <c r="G35" s="41"/>
+      <c r="G35" s="40"/>
       <c r="H35" s="6" t="s">
         <v>119</v>
       </c>
@@ -2544,122 +2547,126 @@
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="47" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="42" t="s">
+    <row r="36" spans="1:9" s="46" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="43"/>
-      <c r="C36" s="43"/>
-      <c r="D36" s="43">
+      <c r="B36" s="42"/>
+      <c r="C36" s="42"/>
+      <c r="D36" s="42">
         <v>226</v>
       </c>
-      <c r="E36" s="44" t="s">
+      <c r="E36" s="43" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="45" t="s">
+      <c r="F36" s="44" t="s">
         <v>166</v>
       </c>
-      <c r="G36" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H36" s="45" t="s">
+      <c r="G36" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H36" s="44" t="s">
         <v>120</v>
       </c>
-      <c r="I36" s="43" t="s">
+      <c r="I36" s="42" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="7" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="16" t="s">
+    <row r="37" spans="1:9" s="46" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="5"/>
-      <c r="C37" s="5"/>
-      <c r="D37" s="5">
+      <c r="B37" s="42"/>
+      <c r="C37" s="42"/>
+      <c r="D37" s="42">
         <v>254</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="49" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="6"/>
-      <c r="G37" s="41"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="5" t="s">
+      <c r="F37" s="44" t="s">
+        <v>168</v>
+      </c>
+      <c r="G37" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H37" s="44"/>
+      <c r="I37" s="42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="47" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A38" s="42" t="s">
+    <row r="38" spans="1:9" s="46" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A38" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="43"/>
-      <c r="C38" s="43"/>
-      <c r="D38" s="43" t="s">
+      <c r="B38" s="42"/>
+      <c r="C38" s="42"/>
+      <c r="D38" s="42" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="44" t="s">
+      <c r="E38" s="43" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="45" t="s">
+      <c r="F38" s="44" t="s">
         <v>167</v>
       </c>
-      <c r="G38" s="46" t="s">
-        <v>134</v>
-      </c>
-      <c r="H38" s="45" t="s">
+      <c r="G38" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="H38" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="I38" s="43" t="s">
+      <c r="I38" s="42" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="34" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A39" s="30" t="s">
+    <row r="39" spans="1:9" s="33" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A39" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="31" t="s">
+      <c r="B39" s="30"/>
+      <c r="C39" s="30"/>
+      <c r="D39" s="30" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="35" t="s">
+      <c r="E39" s="34" t="s">
         <v>59</v>
       </c>
-      <c r="F39" s="33" t="s">
+      <c r="F39" s="32" t="s">
         <v>138</v>
       </c>
-      <c r="G39" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H39" s="33" t="s">
+      <c r="G39" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H39" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="I39" s="31" t="s">
+      <c r="I39" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="34" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A40" s="30" t="s">
+    <row r="40" spans="1:9" s="33" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A40" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="31"/>
-      <c r="C40" s="31"/>
-      <c r="D40" s="31" t="s">
+      <c r="B40" s="30"/>
+      <c r="C40" s="30"/>
+      <c r="D40" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="34" t="s">
         <v>61</v>
       </c>
-      <c r="F40" s="33" t="s">
+      <c r="F40" s="32" t="s">
         <v>139</v>
       </c>
-      <c r="G40" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H40" s="33" t="s">
+      <c r="G40" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H40" s="32" t="s">
         <v>122</v>
       </c>
-      <c r="I40" s="31" t="s">
+      <c r="I40" s="30" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2672,11 +2679,11 @@
       <c r="D41" s="5">
         <v>425</v>
       </c>
-      <c r="E41" s="25" t="s">
+      <c r="E41" s="24" t="s">
         <v>64</v>
       </c>
       <c r="F41" s="6"/>
-      <c r="G41" s="41"/>
+      <c r="G41" s="40"/>
       <c r="H41" s="6" t="s">
         <v>123</v>
       </c>
@@ -2693,7 +2700,7 @@
       <c r="D42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="26" t="s">
+      <c r="E42" s="25" t="s">
         <v>65</v>
       </c>
       <c r="F42" s="4"/>
@@ -2702,53 +2709,53 @@
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="34" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A43" s="30" t="s">
+    <row r="43" spans="1:9" s="33" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A43" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="31"/>
-      <c r="C43" s="31"/>
-      <c r="D43" s="31" t="s">
+      <c r="B43" s="30"/>
+      <c r="C43" s="30"/>
+      <c r="D43" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="35" t="s">
+      <c r="E43" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="38" t="s">
+      <c r="F43" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="G43" s="31" t="s">
-        <v>134</v>
-      </c>
-      <c r="H43" s="33" t="s">
+      <c r="G43" s="30" t="s">
+        <v>134</v>
+      </c>
+      <c r="H43" s="32" t="s">
         <v>124</v>
       </c>
-      <c r="I43" s="31" t="s">
+      <c r="I43" s="30" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="34" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="30" t="s">
+    <row r="44" spans="1:9" s="33" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="31" t="s">
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="35" t="s">
+      <c r="E44" s="34" t="s">
         <v>68</v>
       </c>
-      <c r="F44" s="33" t="s">
+      <c r="F44" s="32" t="s">
         <v>143</v>
       </c>
-      <c r="G44" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H44" s="33" t="s">
+      <c r="G44" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H44" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="I44" s="31" t="s">
+      <c r="I44" s="30" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2761,11 +2768,11 @@
       <c r="D45" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="E45" s="23" t="s">
+      <c r="E45" s="22" t="s">
         <v>70</v>
       </c>
       <c r="F45" s="9"/>
-      <c r="G45" s="39"/>
+      <c r="G45" s="38"/>
       <c r="H45" s="11" t="s">
         <v>71</v>
       </c>
@@ -2773,28 +2780,28 @@
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="34" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A46" s="30" t="s">
+    <row r="46" spans="1:9" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A46" s="29" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="31"/>
-      <c r="C46" s="31"/>
-      <c r="D46" s="31" t="s">
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="36" t="s">
+      <c r="E46" s="35" t="s">
         <v>73</v>
       </c>
-      <c r="F46" s="38" t="s">
+      <c r="F46" s="37" t="s">
         <v>144</v>
       </c>
-      <c r="G46" s="38" t="s">
-        <v>134</v>
-      </c>
-      <c r="H46" s="33" t="s">
+      <c r="G46" s="37" t="s">
+        <v>134</v>
+      </c>
+      <c r="H46" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="30" t="s">
         <v>112</v>
       </c>
     </row>
@@ -2807,7 +2814,7 @@
       </c>
       <c r="C47" s="2"/>
       <c r="D47" s="2"/>
-      <c r="E47" s="27" t="s">
+      <c r="E47" s="26" t="s">
         <v>76</v>
       </c>
       <c r="I47" s="1" t="s">
@@ -2823,7 +2830,7 @@
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="2"/>
-      <c r="E48" s="27" t="s">
+      <c r="E48" s="26" t="s">
         <v>79</v>
       </c>
       <c r="I48" s="1" t="s">
@@ -2839,7 +2846,7 @@
       </c>
       <c r="C49" s="2"/>
       <c r="D49" s="2"/>
-      <c r="E49" s="27" t="s">
+      <c r="E49" s="26" t="s">
         <v>80</v>
       </c>
       <c r="I49" s="1" t="s">
@@ -2855,7 +2862,7 @@
       </c>
       <c r="C50" s="2"/>
       <c r="D50" s="2"/>
-      <c r="E50" s="27" t="s">
+      <c r="E50" s="26" t="s">
         <v>82</v>
       </c>
       <c r="I50" s="1" t="s">
@@ -2871,7 +2878,7 @@
       </c>
       <c r="C51" s="2"/>
       <c r="D51" s="2"/>
-      <c r="E51" s="27" t="s">
+      <c r="E51" s="26" t="s">
         <v>84</v>
       </c>
       <c r="I51" s="1" t="s">
@@ -2889,7 +2896,7 @@
       <c r="D52" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E52" s="27" t="s">
+      <c r="E52" s="26" t="s">
         <v>87</v>
       </c>
       <c r="I52" s="1" t="s">
@@ -2907,7 +2914,7 @@
       <c r="D53" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E53" s="27" t="s">
+      <c r="E53" s="26" t="s">
         <v>89</v>
       </c>
       <c r="I53" s="1" t="s">
@@ -2925,7 +2932,7 @@
       <c r="D54" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E54" s="27" t="s">
+      <c r="E54" s="26" t="s">
         <v>90</v>
       </c>
       <c r="I54" s="1" t="s">
@@ -2941,7 +2948,7 @@
       </c>
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
-      <c r="E55" s="27" t="s">
+      <c r="E55" s="26" t="s">
         <v>91</v>
       </c>
       <c r="I55" s="1" t="s">
@@ -2957,7 +2964,7 @@
       </c>
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
-      <c r="E56" s="27" t="s">
+      <c r="E56" s="26" t="s">
         <v>93</v>
       </c>
       <c r="I56" s="1" t="s">
@@ -2973,7 +2980,7 @@
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
-      <c r="E57" s="27" t="s">
+      <c r="E57" s="26" t="s">
         <v>94</v>
       </c>
       <c r="I57" s="1" t="s">
@@ -2991,7 +2998,7 @@
       <c r="D58" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="E58" s="27" t="s">
+      <c r="E58" s="26" t="s">
         <v>96</v>
       </c>
       <c r="F58" s="3" t="s">
@@ -3012,7 +3019,7 @@
       <c r="D59" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="E59" s="27" t="s">
+      <c r="E59" s="26" t="s">
         <v>99</v>
       </c>
       <c r="I59" s="1" t="s">
@@ -3030,7 +3037,7 @@
       <c r="D60" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E60" s="27" t="s">
+      <c r="E60" s="26" t="s">
         <v>102</v>
       </c>
       <c r="I60" s="1" t="s">
@@ -3048,7 +3055,7 @@
       <c r="D61" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="E61" s="27" t="s">
+      <c r="E61" s="26" t="s">
         <v>104</v>
       </c>
       <c r="I61" s="1" t="s">
@@ -3066,7 +3073,7 @@
       <c r="D62" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="E62" s="27" t="s">
+      <c r="E62" s="26" t="s">
         <v>106</v>
       </c>
       <c r="I62" s="1" t="s">
@@ -3084,7 +3091,7 @@
       <c r="D63" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="E63" s="27" t="s">
+      <c r="E63" s="26" t="s">
         <v>107</v>
       </c>
       <c r="I63" s="1" t="s">
@@ -3102,7 +3109,7 @@
       <c r="D64" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="E64" s="27" t="s">
+      <c r="E64" s="26" t="s">
         <v>111</v>
       </c>
       <c r="I64" s="1" t="s">

</xml_diff>

<commit_message>
Working on Tania's comments.
</commit_message>
<xml_diff>
--- a/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
+++ b/Submissions/2-Comments from internal reviewers/Comments_1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mkh2/github/MaterialExergyPaper2025/Submissions/2-Comments from internal reviewers/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3381750D-2DB6-5B44-9AAA-B3B4FBE47D54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{649BFF51-597A-924B-A785-84B9CE6E9BD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{981245B0-1744-4A2D-8621-ECED626B50B6}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="172">
   <si>
     <t>Commenter</t>
   </si>
@@ -834,6 +834,15 @@
   </si>
   <si>
     <t>Added in chemical exergy section.</t>
+  </si>
+  <si>
+    <t>Address this comment when we pull some results from the Discussion (Section 4) into Results (Section 3).</t>
+  </si>
+  <si>
+    <t>This issue was addressed in re sponse to Laura's comment above.</t>
+  </si>
+  <si>
+    <t>This is a good comment. Thanks!</t>
   </si>
 </sst>
 </file>
@@ -981,9 +990,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1047,9 +1053,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1113,6 +1116,12 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1728,26 +1737,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10161703-9168-4F1F-9C6E-437384505A5D}">
-  <dimension ref="A1:I64"/>
+  <dimension ref="A1:I78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.6640625" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.6640625" style="18" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.1640625" style="27" customWidth="1"/>
-    <col min="6" max="6" width="48.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="36.1640625" style="36" customWidth="1"/>
-    <col min="8" max="8" width="66.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="28"/>
+    <col min="5" max="5" width="61.1640625" style="25" customWidth="1"/>
+    <col min="6" max="6" width="48.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="36.1640625" style="34" customWidth="1"/>
+    <col min="8" max="8" width="66.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.83203125" style="26"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -1759,498 +1768,498 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="36" t="s">
+      <c r="G1" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
+    <row r="2" spans="1:9" s="31" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30" t="s">
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="35" t="s">
+      <c r="E2" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="32" t="s">
+      <c r="F2" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="G2" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H2" s="32" t="s">
+      <c r="G2" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H2" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I2" s="30" t="s">
+      <c r="I2" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="30" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="29" t="s">
+    <row r="3" spans="1:9" s="28" customFormat="1" ht="52" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="30" t="s">
+      <c r="D3" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="30" t="s">
+      <c r="E3" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="47" t="s">
+      <c r="F3" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="G3" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="H3" s="32" t="s">
+      <c r="G3" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="H3" s="30" t="s">
         <v>146</v>
       </c>
-      <c r="I3" s="30" t="s">
+      <c r="I3" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="33" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A4" s="29" t="s">
+    <row r="4" spans="1:9" s="31" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="30"/>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30">
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28">
         <v>48</v>
       </c>
-      <c r="E4" s="35" t="s">
+      <c r="E4" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="32" t="s">
+      <c r="F4" s="30" t="s">
         <v>140</v>
       </c>
-      <c r="G4" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H4" s="32" t="s">
+      <c r="G4" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H4" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="30" t="s">
+      <c r="I4" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="46" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A5" s="41" t="s">
+    <row r="5" spans="1:9" s="44" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A5" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="42"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42">
+      <c r="B5" s="40"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40">
         <v>74</v>
       </c>
-      <c r="E5" s="43" t="s">
+      <c r="E5" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="F5" s="44" t="s">
+      <c r="F5" s="42" t="s">
         <v>151</v>
       </c>
-      <c r="G5" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H5" s="44"/>
-      <c r="I5" s="42" t="s">
+      <c r="G5" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H5" s="42"/>
+      <c r="I5" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="46" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="41" t="s">
+    <row r="6" spans="1:9" s="44" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A6" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40">
         <v>151</v>
       </c>
-      <c r="E6" s="43" t="s">
+      <c r="E6" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="44" t="s">
+      <c r="F6" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="G6" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H6" s="44" t="s">
+      <c r="G6" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H6" s="42" t="s">
         <v>152</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A7" s="41" t="s">
+    <row r="7" spans="1:9" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A7" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="42"/>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42">
+      <c r="B7" s="40"/>
+      <c r="C7" s="40"/>
+      <c r="D7" s="40">
         <v>159</v>
       </c>
-      <c r="E7" s="43" t="s">
+      <c r="E7" s="41" t="s">
         <v>127</v>
       </c>
-      <c r="F7" s="44" t="s">
+      <c r="F7" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H7" s="44"/>
-      <c r="I7" s="42" t="s">
+      <c r="G7" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H7" s="42"/>
+      <c r="I7" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="33" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+    <row r="8" spans="1:9" s="31" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A8" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30" t="s">
+      <c r="B8" s="28"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="35" t="s">
+      <c r="E8" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="F8" s="32" t="s">
+      <c r="F8" s="30" t="s">
         <v>149</v>
       </c>
-      <c r="G8" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="30" t="s">
+      <c r="G8" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H8" s="30"/>
+      <c r="I8" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="33" customFormat="1" ht="176" x14ac:dyDescent="0.2">
-      <c r="A9" s="29" t="s">
+    <row r="9" spans="1:9" s="31" customFormat="1" ht="176" x14ac:dyDescent="0.2">
+      <c r="A9" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30">
+      <c r="B9" s="28"/>
+      <c r="C9" s="28"/>
+      <c r="D9" s="28">
         <v>218</v>
       </c>
-      <c r="E9" s="35" t="s">
+      <c r="E9" s="33" t="s">
         <v>128</v>
       </c>
-      <c r="F9" s="32" t="s">
+      <c r="F9" s="30" t="s">
         <v>150</v>
       </c>
-      <c r="G9" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H9" s="32"/>
-      <c r="I9" s="30" t="s">
+      <c r="G9" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H9" s="30"/>
+      <c r="I9" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="46" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A10" s="41" t="s">
+    <row r="10" spans="1:9" s="44" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A10" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="42"/>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42" t="s">
+      <c r="B10" s="40"/>
+      <c r="C10" s="40"/>
+      <c r="D10" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="43" t="s">
+      <c r="E10" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="F10" s="44" t="s">
+      <c r="F10" s="42" t="s">
         <v>154</v>
       </c>
-      <c r="G10" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H10" s="44"/>
-      <c r="I10" s="42" t="s">
+      <c r="G10" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H10" s="42"/>
+      <c r="I10" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="33" customFormat="1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A11" s="29" t="s">
+    <row r="11" spans="1:9" s="31" customFormat="1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="30"/>
-      <c r="C11" s="30"/>
-      <c r="D11" s="30" t="s">
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="35" t="s">
+      <c r="E11" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="32" t="s">
+      <c r="F11" s="30" t="s">
         <v>141</v>
       </c>
-      <c r="G11" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H11" s="32" t="s">
+      <c r="G11" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H11" s="30" t="s">
         <v>114</v>
       </c>
-      <c r="I11" s="30" t="s">
+      <c r="I11" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+    <row r="12" spans="1:9" s="31" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A12" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30" t="s">
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="35" t="s">
+      <c r="E12" s="33" t="s">
         <v>129</v>
       </c>
-      <c r="F12" s="32" t="s">
+      <c r="F12" s="30" t="s">
         <v>142</v>
       </c>
-      <c r="G12" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H12" s="32"/>
-      <c r="I12" s="30" t="s">
+      <c r="G12" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H12" s="30"/>
+      <c r="I12" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="46" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A13" s="41" t="s">
+    <row r="13" spans="1:9" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A13" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B13" s="42"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42" t="s">
+      <c r="B13" s="40"/>
+      <c r="C13" s="40"/>
+      <c r="D13" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="E13" s="43" t="s">
+      <c r="E13" s="41" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="44" t="s">
+      <c r="F13" s="42" t="s">
         <v>155</v>
       </c>
-      <c r="G13" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H13" s="48"/>
-      <c r="I13" s="42" t="s">
+      <c r="G13" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H13" s="46"/>
+      <c r="I13" s="40" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A14" s="41" t="s">
+    <row r="14" spans="1:9" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A14" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42">
+      <c r="B14" s="40"/>
+      <c r="C14" s="40"/>
+      <c r="D14" s="40">
         <v>438</v>
       </c>
-      <c r="E14" s="43" t="s">
+      <c r="E14" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="44" t="s">
+      <c r="F14" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="G14" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H14" s="44" t="s">
+      <c r="G14" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H14" s="42" t="s">
         <v>156</v>
       </c>
-      <c r="I14" s="42" t="s">
+      <c r="I14" s="40" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="15" spans="1:9" s="46" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A15" s="41" t="s">
+    <row r="15" spans="1:9" s="44" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A15" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42" t="s">
+      <c r="B15" s="40"/>
+      <c r="C15" s="40"/>
+      <c r="D15" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="43" t="s">
+      <c r="E15" s="41" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="44" t="s">
+      <c r="F15" s="42" t="s">
         <v>153</v>
       </c>
-      <c r="G15" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H15" s="44" t="s">
+      <c r="G15" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H15" s="42" t="s">
         <v>157</v>
       </c>
-      <c r="I15" s="42" t="s">
+      <c r="I15" s="40" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="46" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A16" s="41" t="s">
+    <row r="16" spans="1:9" s="44" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A16" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B16" s="42"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42" t="s">
+      <c r="B16" s="40"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40" t="s">
         <v>27</v>
       </c>
-      <c r="E16" s="43" t="s">
+      <c r="E16" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="44" t="s">
+      <c r="F16" s="42" t="s">
         <v>143</v>
       </c>
-      <c r="G16" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H16" s="44" t="s">
+      <c r="G16" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H16" s="42" t="s">
         <v>115</v>
       </c>
-      <c r="I16" s="42" t="s">
+      <c r="I16" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A17" s="41" t="s">
+    <row r="17" spans="1:9" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A17" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="42"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42">
+      <c r="B17" s="40"/>
+      <c r="C17" s="40"/>
+      <c r="D17" s="40">
         <v>487</v>
       </c>
-      <c r="E17" s="43" t="s">
+      <c r="E17" s="41" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="44"/>
-      <c r="G17" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H17" s="44"/>
-      <c r="I17" s="42" t="s">
+      <c r="F17" s="42"/>
+      <c r="G17" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H17" s="42"/>
+      <c r="I17" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="46" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A18" s="41" t="s">
+    <row r="18" spans="1:9" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A18" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B18" s="42"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42" t="s">
+      <c r="B18" s="40"/>
+      <c r="C18" s="40"/>
+      <c r="D18" s="40" t="s">
         <v>30</v>
       </c>
-      <c r="E18" s="43" t="s">
+      <c r="E18" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="44"/>
-      <c r="G18" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H18" s="44" t="s">
+      <c r="F18" s="42"/>
+      <c r="G18" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H18" s="42" t="s">
         <v>158</v>
       </c>
-      <c r="I18" s="42" t="s">
+      <c r="I18" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="46" customFormat="1" ht="68" x14ac:dyDescent="0.2">
-      <c r="A19" s="41" t="s">
+    <row r="19" spans="1:9" s="44" customFormat="1" ht="68" x14ac:dyDescent="0.2">
+      <c r="A19" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="42"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42">
+      <c r="B19" s="40"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40">
         <v>526</v>
       </c>
-      <c r="E19" s="43" t="s">
+      <c r="E19" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="44" t="s">
+      <c r="F19" s="42" t="s">
         <v>159</v>
       </c>
-      <c r="G19" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H19" s="44" t="s">
+      <c r="G19" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H19" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="I19" s="42" t="s">
+      <c r="I19" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="41" t="s">
+    <row r="20" spans="1:9" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A20" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="42"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42">
+      <c r="B20" s="40"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40">
         <v>527</v>
       </c>
-      <c r="E20" s="43" t="s">
+      <c r="E20" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="F20" s="44" t="s">
+      <c r="F20" s="42" t="s">
         <v>160</v>
       </c>
-      <c r="G20" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H20" s="44"/>
-      <c r="I20" s="42" t="s">
+      <c r="G20" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H20" s="42"/>
+      <c r="I20" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="41" t="s">
+    <row r="21" spans="1:9" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A21" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="42"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42">
+      <c r="B21" s="40"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40">
         <v>533</v>
       </c>
-      <c r="E21" s="43" t="s">
+      <c r="E21" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="F21" s="44" t="s">
+      <c r="F21" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="G21" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H21" s="44"/>
-      <c r="I21" s="42" t="s">
+      <c r="G21" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H21" s="42"/>
+      <c r="I21" s="40" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="53" x14ac:dyDescent="0.2">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B22" s="1"/>
@@ -2258,17 +2267,17 @@
       <c r="D22" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E22" s="21" t="s">
+      <c r="E22" s="20" t="s">
         <v>130</v>
       </c>
-      <c r="F22" s="4"/>
-      <c r="H22" s="4"/>
+      <c r="F22" s="3"/>
+      <c r="H22" s="3"/>
       <c r="I22" s="1" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="119" x14ac:dyDescent="0.2">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B23" s="1"/>
@@ -2276,42 +2285,42 @@
       <c r="D23" s="1">
         <v>543</v>
       </c>
-      <c r="E23" s="21" t="s">
+      <c r="E23" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="F23" s="4"/>
-      <c r="H23" s="4"/>
+      <c r="F23" s="3"/>
+      <c r="H23" s="3"/>
       <c r="I23" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="24" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A24" s="41" t="s">
+    <row r="24" spans="1:9" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A24" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B24" s="42"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42" t="s">
+      <c r="B24" s="40"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40" t="s">
         <v>36</v>
       </c>
-      <c r="E24" s="43" t="s">
+      <c r="E24" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="F24" s="42" t="s">
         <v>162</v>
       </c>
-      <c r="G24" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H24" s="44" t="s">
+      <c r="G24" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H24" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="I24" s="42" t="s">
+      <c r="I24" s="40" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="36" x14ac:dyDescent="0.2">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B25" s="1"/>
@@ -2319,61 +2328,61 @@
       <c r="D25" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="E25" s="21" t="s">
+      <c r="E25" s="20" t="s">
         <v>131</v>
       </c>
-      <c r="F25" s="4"/>
-      <c r="H25" s="4"/>
+      <c r="F25" s="3"/>
+      <c r="H25" s="3"/>
       <c r="I25" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A26" s="41" t="s">
+    <row r="26" spans="1:9" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A26" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="42"/>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42">
+      <c r="B26" s="40"/>
+      <c r="C26" s="40"/>
+      <c r="D26" s="40">
         <v>697</v>
       </c>
-      <c r="E26" s="43" t="s">
+      <c r="E26" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="F26" s="44" t="s">
+      <c r="F26" s="42" t="s">
         <v>163</v>
       </c>
-      <c r="G26" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H26" s="44"/>
-      <c r="I26" s="42" t="s">
+      <c r="G26" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H26" s="42"/>
+      <c r="I26" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="46" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A27" s="41" t="s">
+    <row r="27" spans="1:9" s="44" customFormat="1" ht="17" x14ac:dyDescent="0.2">
+      <c r="A27" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42">
+      <c r="B27" s="40"/>
+      <c r="C27" s="40"/>
+      <c r="D27" s="40">
         <v>718</v>
       </c>
-      <c r="E27" s="43" t="s">
+      <c r="E27" s="41" t="s">
         <v>132</v>
       </c>
-      <c r="F27" s="44" t="s">
+      <c r="F27" s="42" t="s">
         <v>164</v>
       </c>
-      <c r="G27" s="45"/>
-      <c r="H27" s="44"/>
-      <c r="I27" s="42" t="s">
+      <c r="G27" s="43"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="40" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="17" x14ac:dyDescent="0.2">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="14" t="s">
         <v>8</v>
       </c>
       <c r="B28" s="1"/>
@@ -2381,318 +2390,318 @@
       <c r="D28" s="1">
         <v>739</v>
       </c>
-      <c r="E28" s="21" t="s">
+      <c r="E28" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="F28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="F28" s="3"/>
+      <c r="H28" s="3"/>
       <c r="I28" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:9" s="33" customFormat="1" ht="48" x14ac:dyDescent="0.2">
-      <c r="A29" s="29" t="s">
+    <row r="29" spans="1:9" s="31" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A29" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B29" s="30"/>
-      <c r="C29" s="30"/>
-      <c r="D29" s="30">
+      <c r="B29" s="28"/>
+      <c r="C29" s="28"/>
+      <c r="D29" s="28">
         <v>18</v>
       </c>
-      <c r="E29" s="31" t="s">
+      <c r="E29" s="29" t="s">
         <v>44</v>
       </c>
-      <c r="F29" s="32" t="s">
+      <c r="F29" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="G29" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H29" s="32" t="s">
+      <c r="G29" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H29" s="30" t="s">
         <v>117</v>
       </c>
-      <c r="I29" s="30" t="s">
+      <c r="I29" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="33" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A30" s="29" t="s">
+    <row r="30" spans="1:9" s="31" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A30" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B30" s="30"/>
-      <c r="C30" s="30"/>
-      <c r="D30" s="30">
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="28">
         <v>51</v>
       </c>
-      <c r="E30" s="34" t="s">
+      <c r="E30" s="32" t="s">
         <v>45</v>
       </c>
-      <c r="F30" s="32" t="s">
+      <c r="F30" s="30" t="s">
         <v>136</v>
       </c>
-      <c r="G30" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H30" s="32"/>
-      <c r="I30" s="30" t="s">
+      <c r="G30" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H30" s="30"/>
+      <c r="I30" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="31" spans="1:9" s="33" customFormat="1" ht="144" x14ac:dyDescent="0.2">
-      <c r="A31" s="29" t="s">
+    <row r="31" spans="1:9" s="31" customFormat="1" ht="144" x14ac:dyDescent="0.2">
+      <c r="A31" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="30" t="s">
+      <c r="B31" s="28"/>
+      <c r="C31" s="28"/>
+      <c r="D31" s="28" t="s">
         <v>43</v>
       </c>
-      <c r="E31" s="34" t="s">
+      <c r="E31" s="32" t="s">
         <v>133</v>
       </c>
-      <c r="F31" s="32" t="s">
+      <c r="F31" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="G31" s="37"/>
-      <c r="H31" s="32" t="s">
+      <c r="G31" s="35"/>
+      <c r="H31" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="I31" s="30" t="s">
+      <c r="I31" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="46" customFormat="1" ht="34" x14ac:dyDescent="0.2">
-      <c r="A32" s="41" t="s">
+    <row r="32" spans="1:9" s="44" customFormat="1" ht="34" x14ac:dyDescent="0.2">
+      <c r="A32" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B32" s="42"/>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42">
+      <c r="B32" s="40"/>
+      <c r="C32" s="40"/>
+      <c r="D32" s="40">
         <v>74</v>
       </c>
-      <c r="E32" s="43" t="s">
+      <c r="E32" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="F32" s="44" t="s">
+      <c r="F32" s="42" t="s">
         <v>165</v>
       </c>
-      <c r="G32" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H32" s="44"/>
-      <c r="I32" s="42" t="s">
+      <c r="G32" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H32" s="42"/>
+      <c r="I32" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="14" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A33" s="18" t="s">
+    <row r="33" spans="1:9" s="13" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A33" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="B33" s="12"/>
-      <c r="C33" s="12"/>
-      <c r="D33" s="12" t="s">
+      <c r="B33" s="11"/>
+      <c r="C33" s="11"/>
+      <c r="D33" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F33" s="13"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="13" t="s">
+      <c r="F33" s="12"/>
+      <c r="G33" s="37"/>
+      <c r="H33" s="12" t="s">
         <v>118</v>
       </c>
-      <c r="I33" s="12" t="s">
+      <c r="I33" s="11" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="33" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A34" s="29" t="s">
+    <row r="34" spans="1:9" s="31" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A34" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B34" s="30"/>
-      <c r="C34" s="30"/>
-      <c r="D34" s="30" t="s">
+      <c r="B34" s="28"/>
+      <c r="C34" s="28"/>
+      <c r="D34" s="28" t="s">
         <v>48</v>
       </c>
-      <c r="E34" s="34" t="s">
+      <c r="E34" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="F34" s="32" t="s">
+      <c r="F34" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="G34" s="37"/>
-      <c r="H34" s="32"/>
-      <c r="I34" s="30" t="s">
+      <c r="G34" s="35"/>
+      <c r="H34" s="30"/>
+      <c r="I34" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="7" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A35" s="16" t="s">
+    <row r="35" spans="1:9" s="6" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A35" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B35" s="5"/>
-      <c r="C35" s="5"/>
-      <c r="D35" s="5" t="s">
+      <c r="B35" s="4"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E35" s="24" t="s">
+      <c r="E35" s="23" t="s">
         <v>54</v>
       </c>
-      <c r="F35" s="6"/>
-      <c r="G35" s="40"/>
-      <c r="H35" s="6" t="s">
+      <c r="F35" s="5"/>
+      <c r="G35" s="38"/>
+      <c r="H35" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="I35" s="5" t="s">
+      <c r="I35" s="4" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="46" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A36" s="41" t="s">
+    <row r="36" spans="1:9" s="44" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A36" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B36" s="42"/>
-      <c r="C36" s="42"/>
-      <c r="D36" s="42">
+      <c r="B36" s="40"/>
+      <c r="C36" s="40"/>
+      <c r="D36" s="40">
         <v>226</v>
       </c>
-      <c r="E36" s="43" t="s">
+      <c r="E36" s="41" t="s">
         <v>55</v>
       </c>
-      <c r="F36" s="44" t="s">
+      <c r="F36" s="42" t="s">
         <v>166</v>
       </c>
-      <c r="G36" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H36" s="44" t="s">
+      <c r="G36" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H36" s="42" t="s">
         <v>120</v>
       </c>
-      <c r="I36" s="42" t="s">
+      <c r="I36" s="40" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="46" customFormat="1" ht="32" x14ac:dyDescent="0.2">
-      <c r="A37" s="41" t="s">
+    <row r="37" spans="1:9" s="44" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="42"/>
-      <c r="C37" s="42"/>
-      <c r="D37" s="42">
+      <c r="B37" s="40"/>
+      <c r="C37" s="40"/>
+      <c r="D37" s="40">
         <v>254</v>
       </c>
-      <c r="E37" s="49" t="s">
+      <c r="E37" s="47" t="s">
         <v>56</v>
       </c>
-      <c r="F37" s="44" t="s">
+      <c r="F37" s="42" t="s">
         <v>168</v>
       </c>
-      <c r="G37" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H37" s="44"/>
-      <c r="I37" s="42" t="s">
+      <c r="G37" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H37" s="42"/>
+      <c r="I37" s="40" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="46" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A38" s="41" t="s">
+    <row r="38" spans="1:9" s="44" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A38" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="B38" s="42"/>
-      <c r="C38" s="42"/>
-      <c r="D38" s="42" t="s">
+      <c r="B38" s="40"/>
+      <c r="C38" s="40"/>
+      <c r="D38" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="E38" s="43" t="s">
+      <c r="E38" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="F38" s="44" t="s">
+      <c r="F38" s="42" t="s">
         <v>167</v>
       </c>
-      <c r="G38" s="45" t="s">
-        <v>134</v>
-      </c>
-      <c r="H38" s="44" t="s">
+      <c r="G38" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H38" s="42" t="s">
         <v>145</v>
       </c>
-      <c r="I38" s="42" t="s">
+      <c r="I38" s="40" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="33" customFormat="1" ht="64" x14ac:dyDescent="0.2">
-      <c r="A39" s="29" t="s">
+    <row r="39" spans="1:9" s="31" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="A39" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B39" s="30"/>
-      <c r="C39" s="30"/>
-      <c r="D39" s="30" t="s">
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="28" t="s">
         <v>58</v>
       </c>
-      <c r="E39" s="34" t="s">
+      <c r="E39" s="32" t="s">
         <v>59</v>
       </c>
-      <c r="F39" s="32" t="s">
+      <c r="F39" s="30" t="s">
         <v>138</v>
       </c>
-      <c r="G39" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H39" s="32" t="s">
+      <c r="G39" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H39" s="30" t="s">
         <v>121</v>
       </c>
-      <c r="I39" s="30" t="s">
+      <c r="I39" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="33" customFormat="1" ht="96" x14ac:dyDescent="0.2">
-      <c r="A40" s="29" t="s">
+    <row r="40" spans="1:9" s="31" customFormat="1" ht="96" x14ac:dyDescent="0.2">
+      <c r="A40" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B40" s="30"/>
-      <c r="C40" s="30"/>
-      <c r="D40" s="30" t="s">
+      <c r="B40" s="28"/>
+      <c r="C40" s="28"/>
+      <c r="D40" s="28" t="s">
         <v>60</v>
       </c>
-      <c r="E40" s="34" t="s">
+      <c r="E40" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="F40" s="32" t="s">
+      <c r="F40" s="30" t="s">
         <v>139</v>
       </c>
-      <c r="G40" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H40" s="32" t="s">
+      <c r="G40" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H40" s="30" t="s">
         <v>122</v>
       </c>
-      <c r="I40" s="30" t="s">
+      <c r="I40" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="16" t="s">
+    <row r="41" spans="1:9" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="B41" s="5"/>
-      <c r="C41" s="5"/>
-      <c r="D41" s="5">
+      <c r="B41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4">
         <v>425</v>
       </c>
-      <c r="E41" s="24" t="s">
+      <c r="E41" s="23" t="s">
         <v>64</v>
       </c>
-      <c r="F41" s="6"/>
-      <c r="G41" s="40"/>
-      <c r="H41" s="6" t="s">
+      <c r="F41" s="5"/>
+      <c r="G41" s="38"/>
+      <c r="H41" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="I41" s="5" t="s">
+      <c r="I41" s="4" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="42" spans="1:9" ht="64" x14ac:dyDescent="0.2">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B42" s="1"/>
@@ -2700,421 +2709,582 @@
       <c r="D42" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="E42" s="25" t="s">
+      <c r="E42" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="F42" s="4"/>
-      <c r="H42" s="4"/>
+      <c r="F42" s="3"/>
+      <c r="H42" s="3" t="s">
+        <v>169</v>
+      </c>
       <c r="I42" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="33" customFormat="1" ht="80" x14ac:dyDescent="0.2">
-      <c r="A43" s="29" t="s">
+    <row r="43" spans="1:9" s="31" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A43" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B43" s="30"/>
-      <c r="C43" s="30"/>
-      <c r="D43" s="30" t="s">
+      <c r="B43" s="28"/>
+      <c r="C43" s="28"/>
+      <c r="D43" s="28" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="34" t="s">
+      <c r="E43" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="F43" s="37" t="s">
+      <c r="F43" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="G43" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="H43" s="32" t="s">
+      <c r="G43" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="H43" s="30" t="s">
         <v>124</v>
       </c>
-      <c r="I43" s="30" t="s">
+      <c r="I43" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="33" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A44" s="29" t="s">
+    <row r="44" spans="1:9" s="31" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A44" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B44" s="30"/>
-      <c r="C44" s="30"/>
-      <c r="D44" s="30" t="s">
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="34" t="s">
+      <c r="E44" s="32" t="s">
         <v>68</v>
       </c>
-      <c r="F44" s="32" t="s">
+      <c r="F44" s="30" t="s">
         <v>143</v>
       </c>
-      <c r="G44" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H44" s="32" t="s">
+      <c r="G44" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H44" s="30" t="s">
         <v>125</v>
       </c>
-      <c r="I44" s="30" t="s">
+      <c r="I44" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="10" customFormat="1" ht="102" x14ac:dyDescent="0.2">
-      <c r="A45" s="17" t="s">
+    <row r="45" spans="1:9" s="9" customFormat="1" ht="102" x14ac:dyDescent="0.2">
+      <c r="A45" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8" t="s">
+      <c r="B45" s="7"/>
+      <c r="C45" s="7"/>
+      <c r="D45" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E45" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="F45" s="9"/>
-      <c r="G45" s="38"/>
-      <c r="H45" s="11" t="s">
+      <c r="F45" s="8"/>
+      <c r="G45" s="36"/>
+      <c r="H45" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="I45" s="8" t="s">
+      <c r="I45" s="7" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="33" customFormat="1" ht="85" x14ac:dyDescent="0.2">
-      <c r="A46" s="29" t="s">
+    <row r="46" spans="1:9" s="31" customFormat="1" ht="85" x14ac:dyDescent="0.2">
+      <c r="A46" s="27" t="s">
         <v>42</v>
       </c>
-      <c r="B46" s="30"/>
-      <c r="C46" s="30"/>
-      <c r="D46" s="30" t="s">
+      <c r="B46" s="28"/>
+      <c r="C46" s="28"/>
+      <c r="D46" s="28" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="35" t="s">
+      <c r="E46" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="F46" s="37" t="s">
+      <c r="F46" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="G46" s="37" t="s">
-        <v>134</v>
-      </c>
-      <c r="H46" s="32" t="s">
+      <c r="G46" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="H46" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="I46" s="30" t="s">
+      <c r="I46" s="28" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A47" s="15" t="s">
+    <row r="47" spans="1:9" s="49" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A47" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="40" t="s">
         <v>75</v>
       </c>
-      <c r="C47" s="2"/>
-      <c r="D47" s="2"/>
-      <c r="E47" s="26" t="s">
+      <c r="C47" s="40"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="48" t="s">
         <v>76</v>
       </c>
-      <c r="I47" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="48" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A48" s="15" t="s">
+      <c r="F47" s="42"/>
+      <c r="G47" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H47" s="42" t="s">
+        <v>171</v>
+      </c>
+      <c r="I47" s="40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" s="49" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A48" s="39" t="s">
         <v>74</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B48" s="40">
         <v>1.2</v>
       </c>
-      <c r="C48" s="2"/>
-      <c r="D48" s="2"/>
-      <c r="E48" s="26" t="s">
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="48" t="s">
         <v>79</v>
       </c>
-      <c r="I48" s="1" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="49" spans="1:9" ht="48" x14ac:dyDescent="0.2">
-      <c r="A49" s="15" t="s">
+      <c r="F48" s="42" t="s">
+        <v>170</v>
+      </c>
+      <c r="G48" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="H48" s="42"/>
+      <c r="I48" s="40" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" s="26" customFormat="1" ht="48" x14ac:dyDescent="0.2">
+      <c r="A49" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B49" s="2">
+      <c r="B49" s="1">
         <v>1.3</v>
       </c>
-      <c r="C49" s="2"/>
-      <c r="D49" s="2"/>
-      <c r="E49" s="26" t="s">
+      <c r="C49" s="1"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="24" t="s">
         <v>80</v>
       </c>
+      <c r="F49" s="3"/>
+      <c r="G49" s="34"/>
+      <c r="H49" s="3"/>
       <c r="I49" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
+    <row r="50" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A50" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="C50" s="2"/>
-      <c r="D50" s="2"/>
-      <c r="E50" s="26" t="s">
+      <c r="C50" s="1"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="24" t="s">
         <v>82</v>
       </c>
+      <c r="F50" s="3"/>
+      <c r="G50" s="34"/>
+      <c r="H50" s="3"/>
       <c r="I50" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A51" s="15" t="s">
+    <row r="51" spans="1:9" s="26" customFormat="1" ht="32" x14ac:dyDescent="0.2">
+      <c r="A51" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C51" s="2"/>
-      <c r="D51" s="2"/>
-      <c r="E51" s="26" t="s">
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="24" t="s">
         <v>84</v>
       </c>
+      <c r="F51" s="3"/>
+      <c r="G51" s="34"/>
+      <c r="H51" s="3"/>
       <c r="I51" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A52" s="15" t="s">
+    <row r="52" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A52" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="2"/>
-      <c r="D52" s="2" t="s">
+      <c r="C52" s="1"/>
+      <c r="D52" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E52" s="26" t="s">
+      <c r="E52" s="24" t="s">
         <v>87</v>
       </c>
+      <c r="F52" s="3"/>
+      <c r="G52" s="34"/>
+      <c r="H52" s="3"/>
       <c r="I52" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="53" spans="1:9" ht="240" x14ac:dyDescent="0.2">
-      <c r="A53" s="15" t="s">
+    <row r="53" spans="1:9" s="26" customFormat="1" ht="240" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C53" s="2"/>
-      <c r="D53" s="2" t="s">
+      <c r="C53" s="1"/>
+      <c r="D53" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E53" s="26" t="s">
+      <c r="E53" s="24" t="s">
         <v>89</v>
       </c>
+      <c r="F53" s="3"/>
+      <c r="G53" s="34"/>
+      <c r="H53" s="3"/>
       <c r="I53" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A54" s="15" t="s">
+    <row r="54" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A54" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B54" s="2" t="s">
+      <c r="B54" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C54" s="2"/>
-      <c r="D54" s="2" t="s">
+      <c r="C54" s="1"/>
+      <c r="D54" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="E54" s="26" t="s">
+      <c r="E54" s="24" t="s">
         <v>90</v>
       </c>
+      <c r="F54" s="3"/>
+      <c r="G54" s="34"/>
+      <c r="H54" s="3"/>
       <c r="I54" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
+    <row r="55" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A55" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C55" s="2"/>
-      <c r="D55" s="2"/>
-      <c r="E55" s="26" t="s">
+      <c r="C55" s="1"/>
+      <c r="D55" s="1"/>
+      <c r="E55" s="24" t="s">
         <v>91</v>
       </c>
+      <c r="F55" s="3"/>
+      <c r="G55" s="34"/>
+      <c r="H55" s="3"/>
       <c r="I55" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
+    <row r="56" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A56" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C56" s="2"/>
-      <c r="D56" s="2"/>
-      <c r="E56" s="26" t="s">
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="24" t="s">
         <v>93</v>
       </c>
+      <c r="F56" s="3"/>
+      <c r="G56" s="34"/>
+      <c r="H56" s="3"/>
       <c r="I56" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="57" spans="1:9" ht="80" x14ac:dyDescent="0.2">
-      <c r="A57" s="15" t="s">
+    <row r="57" spans="1:9" s="26" customFormat="1" ht="80" x14ac:dyDescent="0.2">
+      <c r="A57" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C57" s="2"/>
-      <c r="D57" s="2"/>
-      <c r="E57" s="26" t="s">
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="24" t="s">
         <v>94</v>
       </c>
+      <c r="F57" s="3"/>
+      <c r="G57" s="34"/>
+      <c r="H57" s="3"/>
       <c r="I57" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="58" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A58" s="15" t="s">
+    <row r="58" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A58" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C58" s="2"/>
-      <c r="D58" s="2" t="s">
+      <c r="C58" s="1"/>
+      <c r="D58" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="E58" s="26" t="s">
+      <c r="E58" s="24" t="s">
         <v>96</v>
       </c>
       <c r="F58" s="3" t="s">
         <v>88</v>
       </c>
+      <c r="G58" s="34"/>
+      <c r="H58" s="3"/>
       <c r="I58" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="59" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A59" s="15" t="s">
+    <row r="59" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A59" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C59" s="2"/>
-      <c r="D59" s="2" t="s">
+      <c r="C59" s="1"/>
+      <c r="D59" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E59" s="26" t="s">
+      <c r="E59" s="24" t="s">
         <v>99</v>
       </c>
+      <c r="F59" s="3"/>
+      <c r="G59" s="34"/>
+      <c r="H59" s="3"/>
       <c r="I59" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A60" s="15" t="s">
+    <row r="60" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A60" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B60" s="2" t="s">
+      <c r="B60" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="C60" s="2"/>
-      <c r="D60" s="2" t="s">
+      <c r="C60" s="1"/>
+      <c r="D60" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E60" s="26" t="s">
+      <c r="E60" s="24" t="s">
         <v>102</v>
       </c>
+      <c r="F60" s="3"/>
+      <c r="G60" s="34"/>
+      <c r="H60" s="3"/>
       <c r="I60" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="61" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A61" s="15" t="s">
+    <row r="61" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A61" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="2" t="s">
+      <c r="C61" s="1"/>
+      <c r="D61" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="E61" s="26" t="s">
+      <c r="E61" s="24" t="s">
         <v>104</v>
       </c>
+      <c r="F61" s="3"/>
+      <c r="G61" s="34"/>
+      <c r="H61" s="3"/>
       <c r="I61" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="62" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A62" s="15" t="s">
+    <row r="62" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A62" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B62" s="2">
+      <c r="B62" s="1">
         <v>3.2</v>
       </c>
-      <c r="C62" s="2"/>
-      <c r="D62" s="2" t="s">
+      <c r="C62" s="1"/>
+      <c r="D62" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="E62" s="26" t="s">
+      <c r="E62" s="24" t="s">
         <v>106</v>
       </c>
+      <c r="F62" s="3"/>
+      <c r="G62" s="34"/>
+      <c r="H62" s="3"/>
       <c r="I62" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="63" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A63" s="15" t="s">
+    <row r="63" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A63" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="C63" s="2"/>
-      <c r="D63" s="2" t="s">
+      <c r="C63" s="1"/>
+      <c r="D63" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E63" s="26" t="s">
+      <c r="E63" s="24" t="s">
         <v>107</v>
       </c>
+      <c r="F63" s="3"/>
+      <c r="G63" s="34"/>
+      <c r="H63" s="3"/>
       <c r="I63" s="1" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="64" spans="1:9" ht="16" x14ac:dyDescent="0.2">
-      <c r="A64" s="15" t="s">
+    <row r="64" spans="1:9" s="26" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A64" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="B64" s="2">
+      <c r="B64" s="1">
         <v>4.2</v>
       </c>
-      <c r="C64" s="2"/>
-      <c r="D64" s="2" t="s">
+      <c r="C64" s="1"/>
+      <c r="D64" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="E64" s="26" t="s">
+      <c r="E64" s="24" t="s">
         <v>111</v>
       </c>
+      <c r="F64" s="3"/>
+      <c r="G64" s="34"/>
+      <c r="H64" s="3"/>
       <c r="I64" s="1" t="s">
         <v>78</v>
       </c>
+    </row>
+    <row r="65" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="14"/>
+      <c r="E65" s="19"/>
+      <c r="F65" s="3"/>
+      <c r="G65" s="34"/>
+      <c r="H65" s="3"/>
+    </row>
+    <row r="66" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="14"/>
+      <c r="E66" s="19"/>
+      <c r="F66" s="3"/>
+      <c r="G66" s="34"/>
+      <c r="H66" s="3"/>
+    </row>
+    <row r="67" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="14"/>
+      <c r="E67" s="19"/>
+      <c r="F67" s="3"/>
+      <c r="G67" s="34"/>
+      <c r="H67" s="3"/>
+    </row>
+    <row r="68" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="14"/>
+      <c r="E68" s="19"/>
+      <c r="F68" s="3"/>
+      <c r="G68" s="34"/>
+      <c r="H68" s="3"/>
+    </row>
+    <row r="69" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="14"/>
+      <c r="E69" s="19"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="34"/>
+      <c r="H69" s="3"/>
+    </row>
+    <row r="70" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="14"/>
+      <c r="E70" s="19"/>
+      <c r="F70" s="3"/>
+      <c r="G70" s="34"/>
+      <c r="H70" s="3"/>
+    </row>
+    <row r="71" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="14"/>
+      <c r="E71" s="19"/>
+      <c r="F71" s="3"/>
+      <c r="G71" s="34"/>
+      <c r="H71" s="3"/>
+    </row>
+    <row r="72" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="14"/>
+      <c r="E72" s="19"/>
+      <c r="F72" s="3"/>
+      <c r="G72" s="34"/>
+      <c r="H72" s="3"/>
+    </row>
+    <row r="73" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="14"/>
+      <c r="E73" s="19"/>
+      <c r="F73" s="3"/>
+      <c r="G73" s="34"/>
+      <c r="H73" s="3"/>
+    </row>
+    <row r="74" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="14"/>
+      <c r="E74" s="19"/>
+      <c r="F74" s="3"/>
+      <c r="G74" s="34"/>
+      <c r="H74" s="3"/>
+    </row>
+    <row r="75" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="14"/>
+      <c r="E75" s="19"/>
+      <c r="F75" s="3"/>
+      <c r="G75" s="34"/>
+      <c r="H75" s="3"/>
+    </row>
+    <row r="76" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="14"/>
+      <c r="E76" s="19"/>
+      <c r="F76" s="3"/>
+      <c r="G76" s="34"/>
+      <c r="H76" s="3"/>
+    </row>
+    <row r="77" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="14"/>
+      <c r="E77" s="19"/>
+      <c r="F77" s="3"/>
+      <c r="G77" s="34"/>
+      <c r="H77" s="3"/>
+    </row>
+    <row r="78" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A78" s="14"/>
+      <c r="E78" s="19"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="34"/>
+      <c r="H78" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>